<commit_message>
Table of all num OK
</commit_message>
<xml_diff>
--- a/Example_dataset/Dataset_example_worksheet.xlsx
+++ b/Example_dataset/Dataset_example_worksheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="580" yWindow="700" windowWidth="37240" windowHeight="19220" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="580" yWindow="700" windowWidth="37240" windowHeight="19220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SHENFA" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="295">
   <si>
     <t>Variable 1</t>
   </si>
@@ -487,9 +487,6 @@
     <t>1 cat</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>a1</t>
   </si>
   <si>
@@ -635,9 +632,6 @@
   </si>
   <si>
     <t>see 2num 1 cat with one num ord.</t>
-  </si>
-  <si>
-    <t>distribution of height</t>
   </si>
   <si>
     <t>Story1num</t>
@@ -929,14 +923,20 @@
     <t>18 bubble map</t>
   </si>
   <si>
-    <t>Connection map</t>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>distribution RBNB price</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1218,8 +1218,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1259,6 +1266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF69B3A2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1485,7 +1498,7 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1827,6 +1840,12 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1837,6 +1856,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF69B3A2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3545,7 +3569,7 @@
   <dimension ref="C6:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3555,7 +3579,7 @@
   <sheetData>
     <row r="6" spans="3:11" ht="21" x14ac:dyDescent="0.25">
       <c r="C6" s="101" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D6" s="101"/>
       <c r="E6" s="101"/>
@@ -3568,27 +3592,27 @@
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D16" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3646,7 +3670,7 @@
       <c r="K9" s="68"/>
       <c r="L9" s="68"/>
       <c r="O9" s="87" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="P9" s="68"/>
       <c r="Q9" s="68"/>
@@ -3670,7 +3694,7 @@
       <c r="AI9" s="68"/>
       <c r="AJ9" s="82"/>
       <c r="AL9" s="87" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AM9" s="68"/>
       <c r="AN9" s="68"/>
@@ -3749,22 +3773,22 @@
     </row>
     <row r="16" spans="3:49" ht="26" x14ac:dyDescent="0.3">
       <c r="O16" s="67" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="P16" s="68"/>
       <c r="Q16" s="68"/>
       <c r="S16" s="67" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="T16" s="68"/>
       <c r="U16" s="68"/>
       <c r="W16" s="67" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="X16" s="68"/>
       <c r="Y16" s="68"/>
       <c r="AA16" s="67" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AB16" s="68"/>
       <c r="AC16" s="68"/>
@@ -4230,7 +4254,7 @@
         <v>140</v>
       </c>
       <c r="AQ24" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AT24" s="1" t="s">
         <v>106</v>
@@ -4344,7 +4368,7 @@
         <v>14</v>
       </c>
       <c r="T27" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="U27" s="30" t="s">
         <v>5</v>
@@ -4362,10 +4386,10 @@
         <v>35</v>
       </c>
       <c r="AL27" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AM27" s="113" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AP27" s="1" t="s">
         <v>118</v>
@@ -4385,7 +4409,7 @@
         <v>14</v>
       </c>
       <c r="T28" s="36" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="U28" s="36" t="s">
         <v>6</v>
@@ -4452,7 +4476,7 @@
         <v>1.3</v>
       </c>
       <c r="AL29" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="3:48" x14ac:dyDescent="0.2">
@@ -4475,7 +4499,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AL30" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AT30" s="1" t="s">
         <v>104</v>
@@ -4527,13 +4551,13 @@
         <v>88</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AL32" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AN32" s="72" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="4:46" x14ac:dyDescent="0.2">
@@ -4545,16 +4569,16 @@
         <v>78</v>
       </c>
       <c r="AA33" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AE33" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AL33" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AT33" s="82" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="4:46" x14ac:dyDescent="0.2">
@@ -4562,10 +4586,10 @@
         <v>24</v>
       </c>
       <c r="AA34" s="72" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AE34" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AT34" s="82"/>
     </row>
@@ -4574,10 +4598,10 @@
         <v>25</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="4:46" x14ac:dyDescent="0.2">
@@ -4591,10 +4615,10 @@
         <v>99</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AF37" s="92" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AG37" s="113"/>
     </row>
@@ -4616,7 +4640,7 @@
     </row>
     <row r="40" spans="4:46" x14ac:dyDescent="0.2">
       <c r="O40" s="82" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="P40" s="82"/>
       <c r="Q40" s="82"/>
@@ -4741,33 +4765,33 @@
     </row>
     <row r="46" spans="4:46" x14ac:dyDescent="0.2">
       <c r="D46" s="108" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I46" s="108" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O46" s="108" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="S46" s="108" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="W46" s="108" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AA46" s="108" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AE46" s="108" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AL46" s="108"/>
       <c r="AM46" s="84"/>
       <c r="AP46" s="108" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AT46" s="108" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="4:46" x14ac:dyDescent="0.2">
@@ -4778,7 +4802,7 @@
         <v>54</v>
       </c>
       <c r="O47" s="108" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="S47" s="108" t="s">
         <v>54</v>
@@ -4795,10 +4819,10 @@
       <c r="AL47" s="108"/>
       <c r="AM47" s="84"/>
       <c r="AP47" s="108" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AT47" s="108" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="4:46" x14ac:dyDescent="0.2">
@@ -4873,8 +4897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AM43"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="AB43" sqref="AB43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4991,7 +5015,7 @@
       <c r="S14" s="82"/>
     </row>
     <row r="15" spans="3:37" x14ac:dyDescent="0.2">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="133" t="s">
         <v>95</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -5286,8 +5310,8 @@
       </c>
     </row>
     <row r="20" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C20" s="7" t="s">
-        <v>6</v>
+      <c r="C20" s="134" t="s">
+        <v>294</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>6</v>
@@ -5346,25 +5370,25 @@
     </row>
     <row r="21" spans="3:39" x14ac:dyDescent="0.2">
       <c r="H21" s="107" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I21" s="107"/>
       <c r="J21" s="107"/>
       <c r="K21" s="107"/>
       <c r="P21" s="107" t="s">
+        <v>197</v>
+      </c>
+      <c r="U21" s="107" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y21" s="107" t="s">
         <v>198</v>
       </c>
-      <c r="U21" s="107" t="s">
-        <v>197</v>
-      </c>
-      <c r="Y21" s="107" t="s">
-        <v>199</v>
-      </c>
       <c r="AC21" s="107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AH21" s="107" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="3:39" ht="19" x14ac:dyDescent="0.25">
@@ -5386,7 +5410,7 @@
         <v>145</v>
       </c>
       <c r="AM24" s="104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5411,7 +5435,7 @@
         <v>90</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>90</v>
@@ -5440,7 +5464,7 @@
         <v>142</v>
       </c>
       <c r="AH29" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5448,13 +5472,13 @@
         <v>57</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AH30" s="1" t="s">
         <v>59</v>
       </c>
       <c r="AM30" s="105" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5492,12 +5516,12 @@
         <v>60</v>
       </c>
       <c r="AM36" s="106" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="3:39" x14ac:dyDescent="0.2">
       <c r="AB37" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AM37" s="106"/>
     </row>
@@ -5523,51 +5547,57 @@
     </row>
     <row r="41" spans="3:39" x14ac:dyDescent="0.2">
       <c r="C41" s="108" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I41" s="108" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J41" s="108"/>
       <c r="P41" s="108" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q41" s="108"/>
       <c r="U41" s="108" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB41" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="AB41" s="108" t="s">
-        <v>208</v>
-      </c>
       <c r="AH41" s="108" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="3:39" x14ac:dyDescent="0.2">
       <c r="C42" s="108" t="s">
-        <v>200</v>
+        <v>293</v>
       </c>
       <c r="I42" s="108" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J42" s="108"/>
       <c r="P42" s="108" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q42" s="108"/>
       <c r="U42" s="108" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AB42" s="108" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AH42" s="108" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="P43" s="1" t="s">
-        <v>150</v>
+        <v>292</v>
+      </c>
+      <c r="AB43" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -5615,7 +5645,7 @@
       <c r="D9" s="73"/>
       <c r="E9" s="68"/>
       <c r="H9" s="87" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I9" s="73"/>
       <c r="J9" s="68"/>
@@ -5640,7 +5670,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I12" s="68"/>
       <c r="J12" s="68"/>
@@ -5667,10 +5697,10 @@
         <v>13</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>95</v>
@@ -5705,13 +5735,13 @@
         <v>13</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O15" s="27" t="s">
         <v>13</v>
       </c>
       <c r="P15" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R15" s="27" t="s">
         <v>13</v>
@@ -5734,13 +5764,13 @@
         <v>13</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O16" s="29" t="s">
         <v>13</v>
       </c>
       <c r="P16" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R16" s="29" t="s">
         <v>13</v>
@@ -5757,19 +5787,19 @@
         <v>15</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L17" s="29" t="s">
         <v>13</v>
       </c>
       <c r="M17" s="88" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O17" s="29" t="s">
         <v>13</v>
       </c>
       <c r="P17" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R17" s="29" t="s">
         <v>13</v>
@@ -5783,22 +5813,22 @@
         <v>15</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L18" s="30" t="s">
         <v>14</v>
       </c>
       <c r="M18" s="89" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O18" s="30" t="s">
         <v>14</v>
       </c>
       <c r="P18" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R18" s="30" t="s">
         <v>14</v>
@@ -5812,22 +5842,22 @@
         <v>15</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L19" s="36" t="s">
         <v>14</v>
       </c>
       <c r="M19" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O19" s="36" t="s">
         <v>14</v>
       </c>
       <c r="P19" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R19" s="31" t="s">
         <v>15</v>
@@ -5838,7 +5868,7 @@
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C20" s="107" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.2">
@@ -5856,16 +5886,16 @@
         <v>78</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.2">
@@ -5873,21 +5903,21 @@
         <v>79</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.2">
       <c r="L25" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>106</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.2">
@@ -5898,7 +5928,7 @@
         <v>109</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.2">
@@ -5922,7 +5952,7 @@
         <v>80</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>25</v>
@@ -5953,7 +5983,7 @@
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O34" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
@@ -5975,19 +6005,19 @@
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C40" s="108" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H40" s="108" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L40" s="108" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O40" s="108" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="R40" s="108" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.2">
@@ -6001,7 +6031,7 @@
         <v>54</v>
       </c>
       <c r="O41" s="108" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="R41" s="108" t="s">
         <v>54</v>
@@ -6717,7 +6747,7 @@
   <sheetData>
     <row r="3" spans="3:30" ht="62" x14ac:dyDescent="0.7">
       <c r="H3" s="129" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I3" s="130"/>
       <c r="J3" s="130"/>
@@ -6727,7 +6757,7 @@
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.2">
       <c r="H4" s="132" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I4" s="132"/>
       <c r="J4" s="132"/>
@@ -6758,7 +6788,7 @@
     </row>
     <row r="9" spans="3:30" ht="26" x14ac:dyDescent="0.3">
       <c r="C9" s="87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" s="73"/>
       <c r="E9" s="73"/>
@@ -6767,7 +6797,7 @@
       <c r="H9" s="68"/>
       <c r="I9" s="68"/>
       <c r="L9" s="112" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M9" s="73"/>
       <c r="N9" s="68"/>
@@ -6790,30 +6820,30 @@
     </row>
     <row r="12" spans="3:30" ht="21" x14ac:dyDescent="0.25">
       <c r="C12" s="92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H12" s="92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L12" s="90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M12" s="68"/>
       <c r="N12" s="68"/>
       <c r="P12" s="90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q12" s="68"/>
       <c r="R12" s="68"/>
       <c r="S12" s="68"/>
       <c r="T12" s="68"/>
       <c r="V12" s="90" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="W12" s="68"/>
       <c r="X12" s="68"/>
       <c r="Z12" s="90" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AA12" s="68"/>
       <c r="AB12" s="68"/>
@@ -6831,7 +6861,7 @@
         <v>129</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>129</v>
@@ -6854,22 +6884,22 @@
         <v>1</v>
       </c>
       <c r="L14" s="92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P14" s="92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S14" s="92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V14" s="92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z14" s="92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC14" s="92" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="3:30" x14ac:dyDescent="0.2">
@@ -6904,7 +6934,7 @@
         <v>67</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="T15" s="4" t="s">
         <v>129</v>
@@ -6942,7 +6972,7 @@
         <v>21</v>
       </c>
       <c r="F16" s="93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H16" s="56" t="s">
         <v>15</v>
@@ -7133,7 +7163,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C20" s="92" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F20" s="33"/>
       <c r="L20" s="52" t="s">
@@ -7236,10 +7266,10 @@
         <v>1.3</v>
       </c>
       <c r="L23" s="92" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P23" s="92" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
@@ -7265,7 +7295,7 @@
         <v>96</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P24" s="4" t="s">
         <v>12</v>
@@ -7274,7 +7304,7 @@
         <v>96</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S24" s="4" t="s">
         <v>95</v>
@@ -7283,7 +7313,7 @@
         <v>147</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
@@ -7363,7 +7393,7 @@
         <v>3</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -7412,7 +7442,7 @@
         <v>23</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
@@ -7440,7 +7470,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L30" s="30" t="s">
         <v>14</v>
@@ -7466,7 +7496,7 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L31" s="30" t="s">
         <v>14</v>
@@ -7492,7 +7522,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L32" s="36" t="s">
         <v>14</v>
@@ -7518,10 +7548,10 @@
     </row>
     <row r="34" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D34" s="92" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E34" s="113"/>
       <c r="F34" s="113"/>
@@ -7541,14 +7571,14 @@
     </row>
     <row r="38" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="N38" s="82" t="s">
         <v>82</v>
       </c>
       <c r="O38" s="69"/>
       <c r="P38" s="92" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q38" s="82"/>
     </row>
@@ -7558,18 +7588,18 @@
       </c>
       <c r="O39" s="69"/>
       <c r="P39" s="92" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="3:26" x14ac:dyDescent="0.2">
       <c r="N40" s="82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O40" s="69"/>
     </row>
     <row r="42" spans="3:26" x14ac:dyDescent="0.2">
       <c r="N42" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="3:26" x14ac:dyDescent="0.2">
@@ -7596,13 +7626,13 @@
     </row>
     <row r="45" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C45" s="108" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L45" s="82"/>
       <c r="M45" s="82"/>
       <c r="N45" s="82"/>
       <c r="O45" s="111" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P45" s="82"/>
       <c r="Q45" s="82"/>
@@ -7610,10 +7640,10 @@
       <c r="S45" s="82"/>
       <c r="T45" s="82"/>
       <c r="V45" s="108" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Z45" s="108" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.2">
@@ -7642,34 +7672,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B14:H16"/>
+  <dimension ref="B14:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="109" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E14" s="109" t="s">
-        <v>293</v>
-      </c>
-      <c r="H14" s="109">
-        <v>19</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="108" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E15" s="108" t="s">
-        <v>230</v>
-      </c>
-      <c r="H15" s="108" t="s">
-        <v>294</v>
+        <v>228</v>
+      </c>
+      <c r="H15" s="109">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
@@ -7680,6 +7707,11 @@
         <v>54</v>
       </c>
       <c r="H16" s="108" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="108" t="s">
         <v>54</v>
       </c>
     </row>
@@ -7720,43 +7752,43 @@
         <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="68" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:1" ht="26" x14ac:dyDescent="0.3">
       <c r="A20" s="100" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:1" s="68" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="91" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P44" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q45" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A46" s="100" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q47" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" s="91" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -7832,7 +7864,7 @@
       <c r="AW7" s="82"/>
       <c r="AX7" s="82"/>
       <c r="AZ7" s="87" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="BA7" s="68"/>
       <c r="BB7" s="68"/>
@@ -7974,7 +8006,7 @@
       <c r="CK11" s="68"/>
       <c r="CL11" s="68"/>
       <c r="CO11" s="67" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="CP11" s="68"/>
       <c r="CQ11" s="68"/>
@@ -8017,7 +8049,7 @@
         <v>96</v>
       </c>
       <c r="BB13" s="86" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="BC13" s="114" t="s">
         <v>95</v>
@@ -8054,12 +8086,12 @@
     </row>
     <row r="14" spans="4:101" ht="24" x14ac:dyDescent="0.3">
       <c r="D14" s="74" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E14" s="120"/>
       <c r="F14" s="120"/>
       <c r="M14" s="74" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N14" s="120"/>
       <c r="O14" s="120"/>
@@ -8070,12 +8102,12 @@
       <c r="T14" s="84"/>
       <c r="U14" s="84"/>
       <c r="X14" s="74" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Y14" s="120"/>
       <c r="Z14" s="120"/>
       <c r="AF14" s="74" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AG14" s="120"/>
       <c r="AH14" s="120"/>
@@ -8100,7 +8132,7 @@
         <v>102</v>
       </c>
       <c r="BB14" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="BC14" s="18" t="s">
         <v>2</v>
@@ -8232,7 +8264,7 @@
         <v>103</v>
       </c>
       <c r="BB15" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="BC15" s="6" t="s">
         <v>4</v>
@@ -8368,7 +8400,7 @@
         <v>102</v>
       </c>
       <c r="BB16" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="BC16" s="6" t="s">
         <v>5</v>
@@ -8468,41 +8500,41 @@
     </row>
     <row r="17" spans="4:101" ht="24" x14ac:dyDescent="0.3">
       <c r="D17" s="74" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E17" s="120"/>
       <c r="F17" s="68"/>
       <c r="H17" s="74" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I17" s="120"/>
       <c r="J17" s="68"/>
       <c r="M17" s="74" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N17" s="120"/>
       <c r="Q17" s="74" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="R17" s="120"/>
       <c r="X17" s="74" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="Y17" s="120"/>
       <c r="Z17" s="68"/>
       <c r="AB17" s="74" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AC17" s="120"/>
       <c r="AD17" s="68"/>
       <c r="AE17" s="84"/>
       <c r="AF17" s="74" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AG17" s="120"/>
       <c r="AH17" s="68"/>
       <c r="AJ17" s="74" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AK17" s="120"/>
       <c r="AL17" s="68"/>
@@ -8523,7 +8555,7 @@
         <v>103</v>
       </c>
       <c r="BB17" s="71" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="BC17" s="7" t="s">
         <v>6</v>
@@ -8620,10 +8652,10 @@
         <v>35</v>
       </c>
       <c r="BI18" s="107" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="BR18" s="107" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="BW18" s="30" t="s">
         <v>14</v>
@@ -8644,7 +8676,7 @@
         <v>10</v>
       </c>
       <c r="CE18" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="CO18" s="30" t="s">
         <v>14</v>
@@ -8849,10 +8881,10 @@
         <v>1.3</v>
       </c>
       <c r="AZ20" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="CE20" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -8948,7 +8980,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AZ21" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="BC21" s="72"/>
       <c r="BD21" s="72"/>
@@ -8962,7 +8994,7 @@
         <v>116</v>
       </c>
       <c r="CP21" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9024,7 +9056,7 @@
         <v>13</v>
       </c>
       <c r="AG22" s="127" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AH22" s="6" t="s">
         <v>4</v>
@@ -9051,7 +9083,7 @@
         <v>32</v>
       </c>
       <c r="AZ22" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="BW22" s="72" t="s">
         <v>120</v>
@@ -9060,7 +9092,7 @@
         <v>140</v>
       </c>
       <c r="CE22" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9086,7 +9118,7 @@
         <v>13</v>
       </c>
       <c r="N23" s="122" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O23" s="122" t="s">
         <v>2</v>
@@ -9177,7 +9209,7 @@
         <v>13</v>
       </c>
       <c r="R24" s="122" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S24" s="122" t="s">
         <v>2</v>
@@ -9204,13 +9236,13 @@
         <v>13</v>
       </c>
       <c r="AK24" s="29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AL24" s="29" t="s">
         <v>4</v>
       </c>
       <c r="BW24" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CA24" s="1" t="s">
         <v>60</v>
@@ -9238,7 +9270,7 @@
         <v>14</v>
       </c>
       <c r="N25" s="123" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O25" s="123" t="s">
         <v>6</v>
@@ -9265,7 +9297,7 @@
         <v>14</v>
       </c>
       <c r="AG25" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AH25" s="7" t="s">
         <v>6</v>
@@ -9274,13 +9306,13 @@
         <v>13</v>
       </c>
       <c r="AK25" s="29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AL25" s="29" t="s">
         <v>4</v>
       </c>
       <c r="AP25" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="CA25" s="1" t="s">
         <v>118</v>
@@ -9303,7 +9335,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>5</v>
@@ -9312,7 +9344,7 @@
         <v>14</v>
       </c>
       <c r="N26" s="123" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O26" s="123" t="s">
         <v>6</v>
@@ -9327,7 +9359,7 @@
         <v>6</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AB26" s="30" t="s">
         <v>14</v>
@@ -9348,7 +9380,7 @@
         <v>5</v>
       </c>
       <c r="BW26" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9366,7 +9398,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J27" s="36" t="s">
         <v>6</v>
@@ -9385,7 +9417,7 @@
         <v>14</v>
       </c>
       <c r="R27" s="123" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S27" s="123" t="s">
         <v>6</v>
@@ -9409,7 +9441,7 @@
         <v>5</v>
       </c>
       <c r="CE27" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9431,7 +9463,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="125" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O28" s="125" t="s">
         <v>6</v>
@@ -9440,16 +9472,16 @@
         <v>14</v>
       </c>
       <c r="R28" s="123" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S28" s="123" t="s">
         <v>6</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AF28" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AJ28" s="30" t="s">
         <v>14</v>
@@ -9461,10 +9493,10 @@
         <v>5</v>
       </c>
       <c r="BW28" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="BY28" s="72" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9477,7 +9509,7 @@
         <v>15</v>
       </c>
       <c r="N29" s="125" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O29" s="125" t="s">
         <v>6</v>
@@ -9486,7 +9518,7 @@
         <v>14</v>
       </c>
       <c r="R29" s="123" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="S29" s="123" t="s">
         <v>6</v>
@@ -9501,15 +9533,15 @@
         <v>5</v>
       </c>
       <c r="BW29" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="CE29" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G30" s="84"/>
       <c r="H30" s="84"/>
@@ -9520,7 +9552,7 @@
         <v>15</v>
       </c>
       <c r="N30" s="126" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O30" s="126" t="s">
         <v>6</v>
@@ -9538,19 +9570,19 @@
         <v>99</v>
       </c>
       <c r="AF30" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AJ30" s="30" t="s">
         <v>14</v>
       </c>
       <c r="AK30" s="30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AL30" s="30" t="s">
         <v>6</v>
       </c>
       <c r="CE30" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="CO30" s="1" t="s">
         <v>115</v>
@@ -9566,7 +9598,7 @@
         <v>15</v>
       </c>
       <c r="R31" s="125" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S31" s="125" t="s">
         <v>6</v>
@@ -9575,13 +9607,13 @@
         <v>82</v>
       </c>
       <c r="AB31" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AJ31" s="30" t="s">
         <v>14</v>
       </c>
       <c r="AK31" s="30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AL31" s="30" t="s">
         <v>6</v>
@@ -9589,16 +9621,16 @@
     </row>
     <row r="32" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Q32" s="125" t="s">
         <v>15</v>
       </c>
       <c r="R32" s="125" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="S32" s="125" t="s">
         <v>6</v>
@@ -9607,7 +9639,7 @@
         <v>83</v>
       </c>
       <c r="AB32" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AF32" s="1" t="s">
         <v>99</v>
@@ -9616,7 +9648,7 @@
         <v>14</v>
       </c>
       <c r="AK32" s="30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AL32" s="30" t="s">
         <v>6</v>
@@ -9630,7 +9662,7 @@
         <v>15</v>
       </c>
       <c r="R33" s="125" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S33" s="125" t="s">
         <v>6</v>
@@ -9642,7 +9674,7 @@
         <v>14</v>
       </c>
       <c r="AK33" s="36" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AL33" s="36" t="s">
         <v>6</v>
@@ -9650,16 +9682,16 @@
     </row>
     <row r="34" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="Q34" s="126" t="s">
         <v>15</v>
       </c>
       <c r="R34" s="126" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="S34" s="126" t="s">
         <v>6</v>
@@ -9681,16 +9713,16 @@
         <v>24</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AF36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="AJ36" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9698,7 +9730,7 @@
         <v>25</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF37" s="1" t="s">
         <v>79</v>
@@ -9706,21 +9738,21 @@
     </row>
     <row r="38" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AJ38" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D39" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="BT39" s="113" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="4:72" x14ac:dyDescent="0.2">
@@ -9730,7 +9762,7 @@
     </row>
     <row r="41" spans="4:72" x14ac:dyDescent="0.2">
       <c r="M41" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AJ41" s="1" t="s">
         <v>82</v>
@@ -9743,7 +9775,7 @@
     </row>
     <row r="43" spans="4:72" x14ac:dyDescent="0.2">
       <c r="M43" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="4:72" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
First hist example OK
</commit_message>
<xml_diff>
--- a/Example_dataset/Dataset_example_worksheet.xlsx
+++ b/Example_dataset/Dataset_example_worksheet.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="295">
   <si>
     <t>Variable 1</t>
   </si>
@@ -4895,10 +4895,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AM43"/>
+  <dimension ref="C3:AN43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="AA8" zoomScale="268" zoomScaleNormal="268" zoomScalePageLayoutView="268" workbookViewId="0">
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4911,14 +4911,15 @@
     <col min="12" max="14" width="5" style="1" customWidth="1"/>
     <col min="15" max="23" width="8.5" style="1"/>
     <col min="24" max="24" width="4.5" style="1" customWidth="1"/>
-    <col min="25" max="32" width="8.5" style="1"/>
-    <col min="33" max="33" width="2.83203125" style="1" customWidth="1"/>
-    <col min="34" max="37" width="8.5" style="1"/>
-    <col min="38" max="38" width="1" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="8.5" style="1"/>
+    <col min="25" max="28" width="8.5" style="1"/>
+    <col min="29" max="33" width="7.6640625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="2.83203125" style="1" customWidth="1"/>
+    <col min="35" max="38" width="8.5" style="1"/>
+    <col min="39" max="39" width="8.5" style="1" customWidth="1"/>
+    <col min="40" max="16384" width="8.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:37" ht="62" x14ac:dyDescent="0.7">
+    <row r="3" spans="3:39" ht="62" x14ac:dyDescent="0.7">
       <c r="K3" s="129" t="s">
         <v>130</v>
       </c>
@@ -4928,7 +4929,7 @@
       <c r="O3" s="130"/>
       <c r="P3" s="131"/>
     </row>
-    <row r="9" spans="3:37" ht="26" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:39" ht="26" x14ac:dyDescent="0.3">
       <c r="C9" s="73" t="s">
         <v>131</v>
       </c>
@@ -4968,8 +4969,9 @@
       <c r="AI9" s="68"/>
       <c r="AJ9" s="68"/>
       <c r="AK9" s="68"/>
-    </row>
-    <row r="13" spans="3:37" ht="26" x14ac:dyDescent="0.3">
+      <c r="AL9" s="68"/>
+    </row>
+    <row r="13" spans="3:39" ht="26" x14ac:dyDescent="0.3">
       <c r="H13" s="67" t="s">
         <v>134</v>
       </c>
@@ -4997,14 +4999,14 @@
       </c>
       <c r="AD13" s="68"/>
       <c r="AE13" s="68"/>
-      <c r="AH13" s="67" t="s">
+      <c r="AI13" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="AI13" s="68"/>
       <c r="AJ13" s="68"/>
-      <c r="AK13" s="82"/>
-    </row>
-    <row r="14" spans="3:37" ht="26" x14ac:dyDescent="0.3">
+      <c r="AK13" s="68"/>
+      <c r="AL13" s="82"/>
+    </row>
+    <row r="14" spans="3:39" ht="26" x14ac:dyDescent="0.3">
       <c r="H14" s="81"/>
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
@@ -5014,361 +5016,397 @@
       <c r="R14" s="82"/>
       <c r="S14" s="82"/>
     </row>
-    <row r="15" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:39" x14ac:dyDescent="0.2">
       <c r="C15" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="Q15" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="U15" s="4" t="s">
+      <c r="U15" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="V15" s="5" t="s">
+      <c r="V15" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="W15" s="5" t="s">
+      <c r="W15" s="133" t="s">
         <v>128</v>
       </c>
-      <c r="Y15" s="4" t="s">
+      <c r="Y15" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="Z15" s="5" t="s">
+      <c r="Z15" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="AA15" s="5" t="s">
+      <c r="AA15" s="133" t="s">
         <v>128</v>
       </c>
-      <c r="AC15" s="4" t="s">
+      <c r="AC15" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="AD15" s="5" t="s">
+      <c r="AD15" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="AE15" s="5" t="s">
+      <c r="AE15" s="133" t="s">
         <v>128</v>
       </c>
-      <c r="AF15" s="5" t="s">
+      <c r="AF15" s="133" t="s">
         <v>144</v>
       </c>
-      <c r="AH15" s="4" t="s">
+      <c r="AG15" s="133" t="s">
+        <v>294</v>
+      </c>
+      <c r="AI15" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="AI15" s="5" t="s">
+      <c r="AJ15" s="133" t="s">
         <v>113</v>
       </c>
-      <c r="AJ15" s="5" t="s">
+      <c r="AK15" s="133" t="s">
         <v>128</v>
       </c>
-      <c r="AK15" s="5" t="s">
+      <c r="AL15" s="133" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="16" spans="3:37" x14ac:dyDescent="0.2">
+      <c r="AM15" s="133" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="3:39" x14ac:dyDescent="0.2">
       <c r="C16" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="P16" s="6">
         <v>1</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="Q16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="U16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="V16" s="3" t="s">
+      <c r="V16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="W16" s="3" t="s">
+      <c r="W16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Y16" s="6">
         <v>1</v>
       </c>
-      <c r="Z16" s="3" t="s">
+      <c r="Z16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AA16" s="3" t="s">
+      <c r="AA16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="AC16" s="6">
         <v>1</v>
       </c>
-      <c r="AD16" s="3" t="s">
+      <c r="AD16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AE16" s="3" t="s">
+      <c r="AE16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AF16" s="3" t="s">
+      <c r="AF16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AH16" s="6" t="s">
+      <c r="AG16" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AI16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AI16" s="3" t="s">
+      <c r="AJ16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AJ16" s="3" t="s">
+      <c r="AK16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AK16" s="3" t="s">
+      <c r="AL16" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="AM16" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C17" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="P17" s="6">
         <v>2</v>
       </c>
-      <c r="Q17" s="3" t="s">
+      <c r="Q17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="U17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="V17" s="3" t="s">
+      <c r="V17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="W17" s="3" t="s">
+      <c r="W17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="Y17" s="6">
         <v>2</v>
       </c>
-      <c r="Z17" s="3" t="s">
+      <c r="Z17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AA17" s="3" t="s">
+      <c r="AA17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="AC17" s="6">
         <v>2</v>
       </c>
-      <c r="AD17" s="3" t="s">
+      <c r="AD17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AE17" s="3" t="s">
+      <c r="AE17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AF17" s="3" t="s">
+      <c r="AF17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AH17" s="6" t="s">
+      <c r="AG17" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AI17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AI17" s="3" t="s">
+      <c r="AJ17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AJ17" s="3" t="s">
+      <c r="AK17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AK17" s="3" t="s">
+      <c r="AL17" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="AM17" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="6" t="s">
         <v>9</v>
       </c>
       <c r="P18" s="6">
         <v>3</v>
       </c>
-      <c r="Q18" s="3" t="s">
+      <c r="Q18" s="6" t="s">
         <v>9</v>
       </c>
       <c r="U18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="V18" s="3" t="s">
+      <c r="V18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="W18" s="3" t="s">
+      <c r="W18" s="6" t="s">
         <v>9</v>
       </c>
       <c r="Y18" s="6">
         <v>3</v>
       </c>
-      <c r="Z18" s="3" t="s">
+      <c r="Z18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AA18" s="3" t="s">
+      <c r="AA18" s="6" t="s">
         <v>9</v>
       </c>
       <c r="AC18" s="6">
         <v>3</v>
       </c>
-      <c r="AD18" s="3" t="s">
+      <c r="AD18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AE18" s="3" t="s">
+      <c r="AE18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AF18" s="3" t="s">
+      <c r="AF18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AH18" s="6" t="s">
+      <c r="AG18" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AI18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AI18" s="3" t="s">
+      <c r="AJ18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AJ18" s="3" t="s">
+      <c r="AK18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AK18" s="3" t="s">
+      <c r="AL18" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="AM18" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C19" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="P19" s="6">
         <v>4</v>
       </c>
-      <c r="Q19" s="3" t="s">
+      <c r="Q19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="U19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="V19" s="3" t="s">
+      <c r="V19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="W19" s="3" t="s">
+      <c r="W19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="Y19" s="6">
         <v>4</v>
       </c>
-      <c r="Z19" s="3" t="s">
+      <c r="Z19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AA19" s="3" t="s">
+      <c r="AA19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="AC19" s="6">
         <v>4</v>
       </c>
-      <c r="AD19" s="3" t="s">
+      <c r="AD19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AE19" s="3" t="s">
+      <c r="AE19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AF19" s="3" t="s">
+      <c r="AF19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AH19" s="6" t="s">
+      <c r="AG19" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AI19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AI19" s="3" t="s">
+      <c r="AJ19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AJ19" s="3" t="s">
+      <c r="AK19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AK19" s="3" t="s">
+      <c r="AL19" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="AM19" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C20" s="134" t="s">
         <v>294</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P20" s="7">
-        <v>5</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="V20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y20" s="7">
-        <v>5</v>
-      </c>
-      <c r="Z20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC20" s="7">
-        <v>5</v>
-      </c>
-      <c r="AD20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AI20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK20" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="H20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="I20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="P20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="U20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="V20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="W20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AC20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AD20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AE20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AG20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AI20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AJ20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AK20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AL20" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="AM20" s="134" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="3:40" x14ac:dyDescent="0.2">
       <c r="H21" s="107" t="s">
         <v>231</v>
       </c>
@@ -5387,11 +5425,11 @@
       <c r="AC21" s="107" t="s">
         <v>198</v>
       </c>
-      <c r="AH21" s="107" t="s">
+      <c r="AI21" s="107" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="3:39" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:40" ht="19" x14ac:dyDescent="0.25">
       <c r="H23" s="85" t="s">
         <v>136</v>
       </c>
@@ -5403,17 +5441,17 @@
       <c r="L23" s="68"/>
       <c r="M23" s="68"/>
       <c r="N23" s="68"/>
-      <c r="AH23" s="82"/>
-    </row>
-    <row r="24" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AH24" s="82" t="s">
+      <c r="AI23" s="82"/>
+    </row>
+    <row r="24" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI24" s="82" t="s">
         <v>145</v>
       </c>
-      <c r="AM24" s="104" t="s">
+      <c r="AN24" s="104" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>31</v>
       </c>
@@ -5426,11 +5464,11 @@
       <c r="U25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AH25" s="1" t="s">
+      <c r="AI25" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>90</v>
       </c>
@@ -5443,17 +5481,17 @@
       <c r="U26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AH26" s="82" t="s">
+      <c r="AI26" s="82" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="3:39" s="102" customFormat="1" ht="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AH27" s="103" t="s">
+    <row r="27" spans="3:40" s="102" customFormat="1" ht="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI27" s="103" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="3:39" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:40" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H29" s="1" t="s">
         <v>138</v>
       </c>
@@ -5463,36 +5501,36 @@
       <c r="U29" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AH29" s="1" t="s">
+      <c r="AI29" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="30" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K30" s="1" t="s">
         <v>57</v>
       </c>
       <c r="U30" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="AH30" s="1" t="s">
+      <c r="AI30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AM30" s="105" t="s">
+      <c r="AN30" s="105" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AH31" s="1" t="s">
+    <row r="31" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI31" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AH32" s="1" t="s">
+    <row r="32" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AI32" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="3:39" s="102" customFormat="1" ht="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="3:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:40" s="102" customFormat="1" ht="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P34" s="1" t="s">
         <v>118</v>
       </c>
@@ -5500,7 +5538,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="3:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:40" x14ac:dyDescent="0.2">
       <c r="P35" s="1" t="s">
         <v>140</v>
       </c>
@@ -5508,24 +5546,24 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="3:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:40" x14ac:dyDescent="0.2">
       <c r="P36" s="1" t="s">
         <v>141</v>
       </c>
       <c r="AB36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AM36" s="106" t="s">
+      <c r="AN36" s="106" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="3:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:40" x14ac:dyDescent="0.2">
       <c r="AB37" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AM37" s="106"/>
-    </row>
-    <row r="40" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="AN37" s="106"/>
+    </row>
+    <row r="40" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C40" s="109">
         <v>1</v>
       </c>
@@ -5541,11 +5579,11 @@
       <c r="AB40" s="109">
         <v>5</v>
       </c>
-      <c r="AH40" s="109">
+      <c r="AI40" s="109">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="3:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C41" s="108" t="s">
         <v>199</v>
       </c>
@@ -5563,11 +5601,11 @@
       <c r="AB41" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="AH41" s="108" t="s">
+      <c r="AI41" s="108" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="3:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C42" s="108" t="s">
         <v>293</v>
       </c>
@@ -5585,11 +5623,11 @@
       <c r="AB42" s="108" t="s">
         <v>289</v>
       </c>
-      <c r="AH42" s="108" t="s">
+      <c r="AI42" s="108" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="43" spans="3:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
         <v>292</v>
       </c>
@@ -5605,6 +5643,9 @@
     <mergeCell ref="K3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C16:C19 AI16:AL19 AD16" numberStoredAsText="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Almost all story created
</commit_message>
<xml_diff>
--- a/Example_dataset/Dataset_example_worksheet.xlsx
+++ b/Example_dataset/Dataset_example_worksheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39560" yWindow="720" windowWidth="37240" windowHeight="19220" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2520" yWindow="2000" windowWidth="31840" windowHeight="17620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SHENFA" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="335">
   <si>
     <t>Variable 1</t>
   </si>
@@ -626,9 +626,6 @@
   </si>
   <si>
     <t>story2numNoOrder</t>
-  </si>
-  <si>
-    <t>height men / women</t>
   </si>
   <si>
     <t>story2numOrder</t>
@@ -968,9 +965,6 @@
     <t>undirected Unweighted</t>
   </si>
   <si>
-    <t>Twitter connection of rstat and python people</t>
-  </si>
-  <si>
     <t>Network of co publication?</t>
   </si>
   <si>
@@ -1035,6 +1029,27 @@
   </si>
   <si>
     <t>Arm transfer</t>
+  </si>
+  <si>
+    <t>Rap Songs</t>
+  </si>
+  <si>
+    <t>Publication Network</t>
+  </si>
+  <si>
+    <t>Migration Flow</t>
+  </si>
+  <si>
+    <t>StoryNestedSeveralvalue</t>
+  </si>
+  <si>
+    <t>Perception of probability</t>
+  </si>
+  <si>
+    <t>bike / temperature ?</t>
+  </si>
+  <si>
+    <t>Twitter connection of #rstat</t>
   </si>
 </sst>
 </file>
@@ -3834,7 +3849,7 @@
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.2">
@@ -3844,12 +3859,12 @@
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3859,10 +3874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:AY69"/>
+  <dimension ref="C3:AY69"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3884,16 +3899,6 @@
     <col min="52" max="16384" width="8.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:51" x14ac:dyDescent="0.2">
-      <c r="AU1" s="127" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="2" spans="3:51" x14ac:dyDescent="0.2">
-      <c r="AU2" s="36" t="s">
-        <v>288</v>
-      </c>
-    </row>
     <row r="3" spans="3:51" ht="62" x14ac:dyDescent="0.7">
       <c r="X3" s="62"/>
       <c r="Y3" s="63"/>
@@ -3908,29 +3913,6 @@
       <c r="AF3" s="64"/>
       <c r="AG3" s="63"/>
       <c r="AH3" s="66"/>
-      <c r="AU3" s="36" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="4" spans="3:51" x14ac:dyDescent="0.2">
-      <c r="AU4" s="36" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="5" spans="3:51" x14ac:dyDescent="0.2">
-      <c r="AU5" s="36" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="6" spans="3:51" x14ac:dyDescent="0.2">
-      <c r="AU6" s="36" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="7" spans="3:51" x14ac:dyDescent="0.2">
-      <c r="AU7" s="37" t="s">
-        <v>288</v>
-      </c>
     </row>
     <row r="9" spans="3:51" ht="26" x14ac:dyDescent="0.3">
       <c r="C9" s="54"/>
@@ -3946,7 +3928,7 @@
       <c r="K9" s="54"/>
       <c r="L9" s="54"/>
       <c r="O9" s="73" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P9" s="54"/>
       <c r="Q9" s="54"/>
@@ -3970,7 +3952,7 @@
       <c r="AI9" s="54"/>
       <c r="AJ9" s="68"/>
       <c r="AL9" s="73" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AM9" s="54"/>
       <c r="AN9" s="54"/>
@@ -4053,22 +4035,22 @@
     </row>
     <row r="16" spans="3:51" ht="26" x14ac:dyDescent="0.3">
       <c r="O16" s="53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P16" s="54"/>
       <c r="Q16" s="54"/>
       <c r="S16" s="53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="T16" s="54"/>
       <c r="U16" s="54"/>
       <c r="W16" s="53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="X16" s="54"/>
       <c r="Y16" s="54"/>
       <c r="AA16" s="53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AB16" s="54"/>
       <c r="AC16" s="54"/>
@@ -4102,7 +4084,7 @@
         <v>113</v>
       </c>
       <c r="AO17" s="127" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ17" s="127" t="s">
         <v>12</v>
@@ -4114,7 +4096,7 @@
         <v>113</v>
       </c>
       <c r="AT17" s="127" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AV17" s="127" t="s">
         <v>12</v>
@@ -4126,7 +4108,7 @@
         <v>113</v>
       </c>
       <c r="AY17" s="127" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="3:51" x14ac:dyDescent="0.2">
@@ -4158,7 +4140,7 @@
         <v>7</v>
       </c>
       <c r="AO18" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ18" s="48" t="s">
         <v>13</v>
@@ -4170,7 +4152,7 @@
         <v>7</v>
       </c>
       <c r="AT18" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AV18" s="48" t="s">
         <v>13</v>
@@ -4182,7 +4164,7 @@
         <v>7</v>
       </c>
       <c r="AY18" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="3:51" x14ac:dyDescent="0.2">
@@ -4217,7 +4199,7 @@
         <v>8</v>
       </c>
       <c r="AO19" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ19" s="48" t="s">
         <v>13</v>
@@ -4229,7 +4211,7 @@
         <v>8</v>
       </c>
       <c r="AT19" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AV19" s="117" t="s">
         <v>14</v>
@@ -4241,7 +4223,7 @@
         <v>11</v>
       </c>
       <c r="AY19" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="3:51" x14ac:dyDescent="0.2">
@@ -4273,7 +4255,7 @@
         <v>9</v>
       </c>
       <c r="AO20" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ20" s="48" t="s">
         <v>13</v>
@@ -4285,7 +4267,7 @@
         <v>9</v>
       </c>
       <c r="AT20" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AV20" s="118" t="s">
         <v>15</v>
@@ -4297,21 +4279,21 @@
         <v>98</v>
       </c>
       <c r="AY20" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="3:51" x14ac:dyDescent="0.2">
       <c r="C21" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D21" s="121" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I21" s="117" t="s">
         <v>14</v>
@@ -4357,10 +4339,10 @@
         <v>95</v>
       </c>
       <c r="AE21" s="127" t="s">
+        <v>292</v>
+      </c>
+      <c r="AF21" s="127" t="s">
         <v>293</v>
-      </c>
-      <c r="AF21" s="127" t="s">
-        <v>294</v>
       </c>
       <c r="AG21" s="127" t="s">
         <v>95</v>
@@ -4375,7 +4357,7 @@
         <v>10</v>
       </c>
       <c r="AO21" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ21" s="117" t="s">
         <v>14</v>
@@ -4387,19 +4369,19 @@
         <v>10</v>
       </c>
       <c r="AT21" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AV21" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AW21" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AX21" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AY21" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="3:51" x14ac:dyDescent="0.2">
@@ -4432,7 +4414,7 @@
         <v>13</v>
       </c>
       <c r="X22" s="51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Y22" s="78" t="s">
         <v>2</v>
@@ -4442,7 +4424,7 @@
         <v>13</v>
       </c>
       <c r="AB22" s="51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AC22" s="45" t="s">
         <v>2</v>
@@ -4466,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="AO22" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ22" s="117" t="s">
         <v>14</v>
@@ -4478,21 +4460,21 @@
         <v>10</v>
       </c>
       <c r="AT22" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="3:51" x14ac:dyDescent="0.2">
       <c r="I23" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O23" s="81" t="s">
         <v>13</v>
       </c>
       <c r="P23" s="125" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>4</v>
@@ -4511,7 +4493,7 @@
         <v>13</v>
       </c>
       <c r="X23" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Y23" s="3" t="s">
         <v>4</v>
@@ -4521,7 +4503,7 @@
         <v>13</v>
       </c>
       <c r="AB23" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AC23" s="46" t="s">
         <v>3</v>
@@ -4536,28 +4518,28 @@
         <v>2</v>
       </c>
       <c r="AL23" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AM23" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AN23" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AO23" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ23" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AR23" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AS23" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AT23" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AV23" s="1" t="s">
         <v>126</v>
@@ -4581,7 +4563,7 @@
         <v>13</v>
       </c>
       <c r="T24" s="125" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U24" s="46" t="s">
         <v>4</v>
@@ -4590,7 +4572,7 @@
         <v>14</v>
       </c>
       <c r="X24" s="117" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y24" s="3" t="s">
         <v>5</v>
@@ -4600,7 +4582,7 @@
         <v>13</v>
       </c>
       <c r="AB24" s="138" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AC24" s="46" t="s">
         <v>4</v>
@@ -4623,7 +4605,7 @@
         <v>14</v>
       </c>
       <c r="P25" s="125" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>6</v>
@@ -4642,7 +4624,7 @@
         <v>14</v>
       </c>
       <c r="X25" s="117" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Y25" s="3">
         <v>3.2</v>
@@ -4652,7 +4634,7 @@
         <v>13</v>
       </c>
       <c r="AB25" s="131" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AC25" s="136" t="s">
         <v>23</v>
@@ -4681,13 +4663,13 @@
         <v>21</v>
       </c>
       <c r="O26" s="128" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P26" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q26" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S26" s="117" t="s">
         <v>14</v>
@@ -4699,19 +4681,19 @@
         <v>6</v>
       </c>
       <c r="W26" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="X26" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Y26" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AA26" s="117" t="s">
         <v>14</v>
       </c>
       <c r="AB26" s="49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AC26" s="46" t="s">
         <v>5</v>
@@ -4726,7 +4708,7 @@
         <v>140</v>
       </c>
       <c r="AR26" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AV26" s="1" t="s">
         <v>109</v>
@@ -4749,7 +4731,7 @@
         <v>14</v>
       </c>
       <c r="T27" s="125" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U27" s="46" t="s">
         <v>5</v>
@@ -4758,13 +4740,13 @@
         <v>14</v>
       </c>
       <c r="AB27" s="133" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AC27" s="46" t="s">
         <v>22</v>
       </c>
       <c r="AE27" s="145" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AF27" s="145"/>
       <c r="AL27" s="58" t="s">
@@ -4782,25 +4764,25 @@
         <v>89</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AA28" s="117" t="s">
         <v>14</v>
       </c>
       <c r="AB28" s="49" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AC28" s="46" t="s">
         <v>2</v>
       </c>
       <c r="AD28" s="143" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AE28" s="144"/>
       <c r="AF28" s="127" t="s">
@@ -4835,7 +4817,7 @@
         <v>14</v>
       </c>
       <c r="AB29" s="50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AC29" s="47" t="s">
         <v>6</v>
@@ -4853,10 +4835,10 @@
         <v>1.3</v>
       </c>
       <c r="AL29" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AM29" s="95" t="s">
         <v>244</v>
-      </c>
-      <c r="AM29" s="95" t="s">
-        <v>245</v>
       </c>
       <c r="AQ29" s="1" t="s">
         <v>118</v>
@@ -4917,7 +4899,7 @@
         <v>32</v>
       </c>
       <c r="AL31" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AV31" s="1" t="s">
         <v>104</v>
@@ -4937,10 +4919,10 @@
         <v>88</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AL32" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AV32" s="1" t="s">
         <v>105</v>
@@ -4955,7 +4937,7 @@
         <v>78</v>
       </c>
       <c r="AA33" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE33" s="1" t="s">
         <v>163</v>
@@ -4967,19 +4949,19 @@
         <v>24</v>
       </c>
       <c r="AA34" s="58" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AE34" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AL34" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AN34" s="58" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AV34" s="68" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="4:48" x14ac:dyDescent="0.2">
@@ -4987,13 +4969,13 @@
         <v>25</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AE35" s="1" t="s">
         <v>173</v>
       </c>
       <c r="AL35" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AV35" s="68"/>
     </row>
@@ -5008,10 +4990,10 @@
         <v>99</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF37" s="76" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AG37" s="95"/>
     </row>
@@ -5033,7 +5015,7 @@
     </row>
     <row r="40" spans="4:48" x14ac:dyDescent="0.2">
       <c r="O40" s="68" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P40" s="68"/>
       <c r="Q40" s="68"/>
@@ -5158,75 +5140,71 @@
     </row>
     <row r="46" spans="4:48" x14ac:dyDescent="0.2">
       <c r="D46" s="90" t="s">
+        <v>203</v>
+      </c>
+      <c r="I46" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="I46" s="90" t="s">
-        <v>205</v>
-      </c>
       <c r="O46" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="S46" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="S46" s="90" t="s">
-        <v>209</v>
-      </c>
       <c r="W46" s="90" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA46" s="90" t="s">
+        <v>331</v>
+      </c>
+      <c r="AE46" s="90" t="s">
         <v>215</v>
       </c>
-      <c r="AA46" s="90" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE46" s="90" t="s">
-        <v>216</v>
+      <c r="AH46" s="90" t="s">
+        <v>334</v>
       </c>
       <c r="AL46" s="90"/>
       <c r="AM46" s="70"/>
       <c r="AQ46" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AV46" s="90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="4:48" x14ac:dyDescent="0.2">
       <c r="D47" s="90" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I47" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="O47" s="90" t="s">
-        <v>207</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="O47" s="90"/>
       <c r="S47" s="90" t="s">
         <v>54</v>
       </c>
       <c r="W47" s="90" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AA47" s="90" t="s">
         <v>54</v>
       </c>
       <c r="AE47" s="161" t="s">
-        <v>302</v>
-      </c>
-      <c r="AH47" s="90" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="AL47" s="90"/>
       <c r="AM47" s="70"/>
       <c r="AQ47" s="90" t="s">
-        <v>199</v>
-      </c>
-      <c r="AV47" s="90" t="s">
-        <v>207</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="AV47" s="90"/>
     </row>
     <row r="48" spans="4:48" x14ac:dyDescent="0.2">
       <c r="AE48" s="161" t="s">
+        <v>302</v>
+      </c>
+      <c r="AH48" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="AH48" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="AM48" s="70"/>
     </row>
@@ -5235,18 +5213,18 @@
     </row>
     <row r="50" spans="26:39" x14ac:dyDescent="0.2">
       <c r="AE50" s="161" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AM50" s="70"/>
     </row>
     <row r="51" spans="26:39" x14ac:dyDescent="0.2">
       <c r="AE51" s="161" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="26:39" x14ac:dyDescent="0.2">
       <c r="AH53" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="61" spans="26:39" x14ac:dyDescent="0.2">
@@ -5316,8 +5294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AN43"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="Q5" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="AI43" sqref="AI43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5482,7 +5460,7 @@
         <v>144</v>
       </c>
       <c r="AG15" s="111" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AI15" s="111" t="s">
         <v>95</v>
@@ -5497,7 +5475,7 @@
         <v>144</v>
       </c>
       <c r="AM15" s="111" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="3:39" x14ac:dyDescent="0.2">
@@ -5547,7 +5525,7 @@
         <v>7</v>
       </c>
       <c r="AG16" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AI16" s="6" t="s">
         <v>2</v>
@@ -5562,7 +5540,7 @@
         <v>7</v>
       </c>
       <c r="AM16" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="3:40" x14ac:dyDescent="0.2">
@@ -5612,7 +5590,7 @@
         <v>8</v>
       </c>
       <c r="AG17" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AI17" s="6" t="s">
         <v>3</v>
@@ -5627,7 +5605,7 @@
         <v>8</v>
       </c>
       <c r="AM17" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="3:40" x14ac:dyDescent="0.2">
@@ -5677,7 +5655,7 @@
         <v>9</v>
       </c>
       <c r="AG18" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AI18" s="6" t="s">
         <v>4</v>
@@ -5692,7 +5670,7 @@
         <v>9</v>
       </c>
       <c r="AM18" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="3:40" x14ac:dyDescent="0.2">
@@ -5742,7 +5720,7 @@
         <v>10</v>
       </c>
       <c r="AG19" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AI19" s="6" t="s">
         <v>5</v>
@@ -5757,77 +5735,77 @@
         <v>10</v>
       </c>
       <c r="AM19" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="V20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="W20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Y20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Z20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AA20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AC20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AD20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AE20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AG20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AI20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AJ20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AK20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AL20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AM20" s="112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="3:40" x14ac:dyDescent="0.2">
       <c r="H21" s="89" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I21" s="89"/>
       <c r="J21" s="89"/>
@@ -5921,7 +5899,7 @@
         <v>142</v>
       </c>
       <c r="AI29" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5929,7 +5907,7 @@
         <v>57</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AI30" s="1" t="s">
         <v>59</v>
@@ -5978,7 +5956,7 @@
     </row>
     <row r="37" spans="3:40" x14ac:dyDescent="0.2">
       <c r="AB37" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AN37" s="88"/>
     </row>
@@ -6011,50 +5989,53 @@
       </c>
       <c r="J41" s="90"/>
       <c r="P41" s="90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q41" s="90"/>
       <c r="U41" s="90" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AB41" s="90" t="s">
+        <v>201</v>
+      </c>
+      <c r="AI41" s="90" t="s">
         <v>202</v>
-      </c>
-      <c r="AI41" s="90" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="42" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C42" s="90" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I42" s="90" t="s">
-        <v>197</v>
+        <v>333</v>
       </c>
       <c r="J42" s="90"/>
       <c r="P42" s="90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q42" s="90"/>
       <c r="U42" s="90" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB42" s="90" t="s">
+        <v>284</v>
+      </c>
+      <c r="AI42" s="90" t="s">
         <v>218</v>
-      </c>
-      <c r="AB42" s="90" t="s">
-        <v>285</v>
-      </c>
-      <c r="AI42" s="90" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="43" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="AB43" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -6073,8 +6054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:T156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A17" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14:S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6105,7 +6086,7 @@
       <c r="D9" s="59"/>
       <c r="E9" s="54"/>
       <c r="H9" s="73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I9" s="59"/>
       <c r="J9" s="54"/>
@@ -6157,10 +6138,10 @@
         <v>13</v>
       </c>
       <c r="H14" s="111" t="s">
+        <v>219</v>
+      </c>
+      <c r="J14" s="111" t="s">
         <v>220</v>
-      </c>
-      <c r="J14" s="111" t="s">
-        <v>221</v>
       </c>
       <c r="L14" s="111" t="s">
         <v>95</v>
@@ -6270,7 +6251,7 @@
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C18" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>154</v>
@@ -6299,10 +6280,10 @@
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.2">
       <c r="H19" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L19" s="117" t="s">
         <v>14</v>
@@ -6328,22 +6309,22 @@
         <v>191</v>
       </c>
       <c r="L20" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M20" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O20" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P20" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R20" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S20" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.2">
@@ -6427,7 +6408,7 @@
         <v>80</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>25</v>
@@ -6458,7 +6439,7 @@
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O34" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
@@ -6480,33 +6461,33 @@
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C40" s="90" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H40" s="90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L40" s="90" t="s">
+        <v>214</v>
+      </c>
+      <c r="O40" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="R40" s="90" t="s">
         <v>215</v>
-      </c>
-      <c r="O40" s="90" t="s">
-        <v>208</v>
-      </c>
-      <c r="R40" s="90" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C41" s="90" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H41" s="90" t="s">
-        <v>54</v>
+        <v>328</v>
       </c>
       <c r="L41" s="90" t="s">
         <v>54</v>
       </c>
       <c r="O41" s="90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R41" s="90" t="s">
         <v>54</v>
@@ -7205,8 +7186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AD47"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:E17"/>
+    <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7230,7 +7211,7 @@
   <sheetData>
     <row r="3" spans="3:30" ht="62" x14ac:dyDescent="0.7">
       <c r="H3" s="113" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I3" s="114"/>
       <c r="J3" s="114"/>
@@ -7280,7 +7261,7 @@
       <c r="H9" s="54"/>
       <c r="I9" s="54"/>
       <c r="L9" s="94" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M9" s="59"/>
       <c r="N9" s="54"/>
@@ -7321,7 +7302,7 @@
       <c r="S12" s="54"/>
       <c r="T12" s="54"/>
       <c r="V12" s="74" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="W12" s="54"/>
       <c r="X12" s="54"/>
@@ -7335,10 +7316,10 @@
     </row>
     <row r="13" spans="3:30" x14ac:dyDescent="0.2">
       <c r="C13" s="127" t="s">
+        <v>292</v>
+      </c>
+      <c r="D13" s="127" t="s">
         <v>293</v>
-      </c>
-      <c r="D13" s="127" t="s">
-        <v>294</v>
       </c>
       <c r="E13" s="127" t="s">
         <v>95</v>
@@ -7420,7 +7401,7 @@
         <v>171</v>
       </c>
       <c r="T15" s="127" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V15" s="127" t="s">
         <v>66</v>
@@ -7555,7 +7536,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C18" s="150" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D18" s="150"/>
       <c r="E18" s="150"/>
@@ -7678,7 +7659,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C21" s="145" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D21" s="145"/>
       <c r="L21" s="49" t="s">
@@ -7711,7 +7692,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B22" s="162" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C22" s="163"/>
       <c r="D22" s="127" t="s">
@@ -7730,31 +7711,31 @@
         <v>129</v>
       </c>
       <c r="L22" s="50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M22" s="152" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P22" s="50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q22" s="152" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="V22" s="50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="W22" s="152" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="X22" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Z22" s="50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AA22" s="152" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
@@ -7844,7 +7825,7 @@
         <v>96</v>
       </c>
       <c r="N25" s="127" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P25" s="127" t="s">
         <v>12</v>
@@ -7853,10 +7834,10 @@
         <v>96</v>
       </c>
       <c r="R25" s="127" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S25" s="127" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Z25" s="76"/>
     </row>
@@ -7868,7 +7849,7 @@
         <v>27</v>
       </c>
       <c r="N26" s="45" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P26" s="51" t="s">
         <v>13</v>
@@ -7877,7 +7858,7 @@
         <v>27</v>
       </c>
       <c r="R26" s="45" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S26" s="45" t="s">
         <v>2</v>
@@ -7894,7 +7875,7 @@
         <v>27</v>
       </c>
       <c r="N27" s="136" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P27" s="48" t="s">
         <v>13</v>
@@ -7903,7 +7884,7 @@
         <v>27</v>
       </c>
       <c r="R27" s="136" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S27" s="46" t="s">
         <v>3</v>
@@ -7917,7 +7898,7 @@
         <v>28</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P28" s="48" t="s">
         <v>13</v>
@@ -7926,7 +7907,7 @@
         <v>28</v>
       </c>
       <c r="R28" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S28" s="46" t="s">
         <v>4</v>
@@ -7943,7 +7924,7 @@
         <v>28</v>
       </c>
       <c r="N29" s="135" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P29" s="131" t="s">
         <v>13</v>
@@ -7952,7 +7933,7 @@
         <v>28</v>
       </c>
       <c r="R29" s="135" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S29" s="136" t="s">
         <v>23</v>
@@ -7969,7 +7950,7 @@
         <v>29</v>
       </c>
       <c r="N30" s="157" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P30" s="117" t="s">
         <v>14</v>
@@ -7978,7 +7959,7 @@
         <v>29</v>
       </c>
       <c r="R30" s="157" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S30" s="46" t="s">
         <v>5</v>
@@ -7995,7 +7976,7 @@
         <v>29</v>
       </c>
       <c r="N31" s="136" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P31" s="117" t="s">
         <v>14</v>
@@ -8004,7 +7985,7 @@
         <v>29</v>
       </c>
       <c r="R31" s="136" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S31" s="46" t="s">
         <v>22</v>
@@ -8021,7 +8002,7 @@
         <v>30</v>
       </c>
       <c r="N32" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P32" s="117" t="s">
         <v>14</v>
@@ -8030,7 +8011,7 @@
         <v>30</v>
       </c>
       <c r="R32" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S32" s="46" t="s">
         <v>2</v>
@@ -8044,7 +8025,7 @@
         <v>30</v>
       </c>
       <c r="N33" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P33" s="122" t="s">
         <v>14</v>
@@ -8053,7 +8034,7 @@
         <v>30</v>
       </c>
       <c r="R33" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S33" s="47" t="s">
         <v>6</v>
@@ -8061,10 +8042,10 @@
     </row>
     <row r="34" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D34" s="76" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E34" s="95"/>
       <c r="F34" s="95"/>
@@ -8083,7 +8064,7 @@
     </row>
     <row r="38" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q38" s="68"/>
     </row>
@@ -8114,7 +8095,7 @@
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.2">
       <c r="N43" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="3:26" x14ac:dyDescent="0.2">
@@ -8130,7 +8111,7 @@
     </row>
     <row r="45" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C45" s="90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L45" s="75"/>
       <c r="M45" s="75"/>
@@ -8144,21 +8125,21 @@
       <c r="S45" s="75"/>
       <c r="T45" s="75"/>
       <c r="V45" s="90" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z45" s="90" t="s">
         <v>223</v>
-      </c>
-      <c r="Z45" s="90" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C46" s="90" t="s">
-        <v>54</v>
+        <v>329</v>
       </c>
       <c r="L46" s="68"/>
       <c r="M46" s="68"/>
       <c r="N46" s="68"/>
       <c r="O46" s="93" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P46" s="68"/>
       <c r="Q46" s="68"/>
@@ -8173,8 +8154,11 @@
       </c>
     </row>
     <row r="47" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="C47" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="O47" s="90" t="s">
-        <v>54</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -8208,37 +8192,37 @@
   <sheetData>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="127" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C6" s="127" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E6" s="127" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F6" s="127" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G6" s="127" t="s">
         <v>129</v>
       </c>
       <c r="J6" s="127" t="s">
+        <v>309</v>
+      </c>
+      <c r="K6" s="127" t="s">
+        <v>312</v>
+      </c>
+      <c r="L6" s="127" t="s">
+        <v>310</v>
+      </c>
+      <c r="M6" s="127" t="s">
         <v>311</v>
       </c>
-      <c r="K6" s="127" t="s">
+      <c r="O6" s="127" t="s">
+        <v>313</v>
+      </c>
+      <c r="P6" s="127" t="s">
         <v>314</v>
-      </c>
-      <c r="L6" s="127" t="s">
-        <v>312</v>
-      </c>
-      <c r="M6" s="127" t="s">
-        <v>313</v>
-      </c>
-      <c r="O6" s="127" t="s">
-        <v>315</v>
-      </c>
-      <c r="P6" s="127" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
@@ -8270,7 +8254,7 @@
         <v>140</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P7" s="35">
         <v>23</v>
@@ -8305,7 +8289,7 @@
         <v>142.30000000000001</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P8" s="36">
         <v>12</v>
@@ -8340,7 +8324,7 @@
         <v>123.8</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="P9" s="36">
         <v>9</v>
@@ -8375,7 +8359,7 @@
         <v>126</v>
       </c>
       <c r="O10" s="47" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P10" s="37">
         <v>10</v>
@@ -8388,27 +8372,27 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="91" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E19" s="91" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J19" s="91">
         <v>19</v>
       </c>
       <c r="O19" s="90" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="90" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E20" s="90" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J20" s="90" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O20" s="90" t="s">
         <v>54</v>
@@ -8427,20 +8411,20 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -8492,31 +8476,31 @@
     <row r="28" spans="1:1" s="54" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="75" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P44" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q45" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A46" s="82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q47" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" s="75" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -8592,7 +8576,7 @@
       <c r="AW7" s="68"/>
       <c r="AX7" s="68"/>
       <c r="AZ7" s="73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BA7" s="54"/>
       <c r="BB7" s="54"/>
@@ -8734,7 +8718,7 @@
       <c r="CK11" s="54"/>
       <c r="CL11" s="54"/>
       <c r="CO11" s="53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="CP11" s="54"/>
       <c r="CQ11" s="54"/>
@@ -8777,7 +8761,7 @@
         <v>96</v>
       </c>
       <c r="BB13" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BC13" s="96" t="s">
         <v>95</v>
@@ -8814,12 +8798,12 @@
     </row>
     <row r="14" spans="4:101" ht="24" x14ac:dyDescent="0.3">
       <c r="D14" s="60" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E14" s="102"/>
       <c r="F14" s="102"/>
       <c r="M14" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N14" s="102"/>
       <c r="O14" s="102"/>
@@ -8830,12 +8814,12 @@
       <c r="T14" s="70"/>
       <c r="U14" s="70"/>
       <c r="X14" s="60" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Y14" s="102"/>
       <c r="Z14" s="102"/>
       <c r="AF14" s="60" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AG14" s="102"/>
       <c r="AH14" s="102"/>
@@ -8860,7 +8844,7 @@
         <v>102</v>
       </c>
       <c r="BB14" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BC14" s="18" t="s">
         <v>2</v>
@@ -8992,7 +8976,7 @@
         <v>103</v>
       </c>
       <c r="BB15" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BC15" s="6" t="s">
         <v>4</v>
@@ -9128,7 +9112,7 @@
         <v>102</v>
       </c>
       <c r="BB16" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BC16" s="6" t="s">
         <v>5</v>
@@ -9228,41 +9212,41 @@
     </row>
     <row r="17" spans="4:101" ht="24" x14ac:dyDescent="0.3">
       <c r="D17" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E17" s="102"/>
       <c r="F17" s="54"/>
       <c r="H17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I17" s="102"/>
       <c r="J17" s="54"/>
       <c r="M17" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N17" s="102"/>
       <c r="Q17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R17" s="102"/>
       <c r="X17" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Y17" s="102"/>
       <c r="Z17" s="54"/>
       <c r="AB17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AC17" s="102"/>
       <c r="AD17" s="54"/>
       <c r="AE17" s="70"/>
       <c r="AF17" s="60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AG17" s="102"/>
       <c r="AH17" s="54"/>
       <c r="AJ17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AK17" s="102"/>
       <c r="AL17" s="54"/>
@@ -9283,7 +9267,7 @@
         <v>103</v>
       </c>
       <c r="BB17" s="57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BC17" s="7" t="s">
         <v>6</v>
@@ -9380,10 +9364,10 @@
         <v>35</v>
       </c>
       <c r="BI18" s="89" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="BR18" s="89" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BW18" s="30" t="s">
         <v>14</v>
@@ -9404,7 +9388,7 @@
         <v>10</v>
       </c>
       <c r="CE18" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="CO18" s="30" t="s">
         <v>14</v>
@@ -9609,10 +9593,10 @@
         <v>1.3</v>
       </c>
       <c r="AZ20" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="CE20" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9708,7 +9692,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AZ21" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="BC21" s="58"/>
       <c r="BD21" s="58"/>
@@ -9722,7 +9706,7 @@
         <v>116</v>
       </c>
       <c r="CP21" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9784,7 +9768,7 @@
         <v>13</v>
       </c>
       <c r="AG22" s="109" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AH22" s="6" t="s">
         <v>4</v>
@@ -9811,7 +9795,7 @@
         <v>32</v>
       </c>
       <c r="AZ22" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="BW22" s="58" t="s">
         <v>120</v>
@@ -9820,7 +9804,7 @@
         <v>140</v>
       </c>
       <c r="CE22" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9846,7 +9830,7 @@
         <v>13</v>
       </c>
       <c r="N23" s="104" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O23" s="104" t="s">
         <v>2</v>
@@ -9937,7 +9921,7 @@
         <v>13</v>
       </c>
       <c r="R24" s="104" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S24" s="104" t="s">
         <v>2</v>
@@ -9964,13 +9948,13 @@
         <v>13</v>
       </c>
       <c r="AK24" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL24" s="29" t="s">
         <v>4</v>
       </c>
       <c r="BW24" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="CA24" s="1" t="s">
         <v>60</v>
@@ -9998,7 +9982,7 @@
         <v>14</v>
       </c>
       <c r="N25" s="105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O25" s="105" t="s">
         <v>6</v>
@@ -10025,7 +10009,7 @@
         <v>14</v>
       </c>
       <c r="AG25" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AH25" s="7" t="s">
         <v>6</v>
@@ -10034,13 +10018,13 @@
         <v>13</v>
       </c>
       <c r="AK25" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL25" s="29" t="s">
         <v>4</v>
       </c>
       <c r="AP25" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="CA25" s="1" t="s">
         <v>118</v>
@@ -10063,7 +10047,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>5</v>
@@ -10072,7 +10056,7 @@
         <v>14</v>
       </c>
       <c r="N26" s="105" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O26" s="105" t="s">
         <v>6</v>
@@ -10087,7 +10071,7 @@
         <v>6</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB26" s="30" t="s">
         <v>14</v>
@@ -10108,7 +10092,7 @@
         <v>5</v>
       </c>
       <c r="BW26" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10126,7 +10110,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J27" s="34" t="s">
         <v>6</v>
@@ -10145,7 +10129,7 @@
         <v>14</v>
       </c>
       <c r="R27" s="105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S27" s="105" t="s">
         <v>6</v>
@@ -10169,7 +10153,7 @@
         <v>5</v>
       </c>
       <c r="CE27" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10191,7 +10175,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O28" s="107" t="s">
         <v>6</v>
@@ -10200,16 +10184,16 @@
         <v>14</v>
       </c>
       <c r="R28" s="105" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S28" s="105" t="s">
         <v>6</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AF28" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AJ28" s="30" t="s">
         <v>14</v>
@@ -10221,10 +10205,10 @@
         <v>5</v>
       </c>
       <c r="BW28" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="BY28" s="58" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10237,7 +10221,7 @@
         <v>15</v>
       </c>
       <c r="N29" s="107" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O29" s="107" t="s">
         <v>6</v>
@@ -10246,7 +10230,7 @@
         <v>14</v>
       </c>
       <c r="R29" s="105" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="S29" s="105" t="s">
         <v>6</v>
@@ -10261,15 +10245,15 @@
         <v>5</v>
       </c>
       <c r="BW29" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="CE29" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G30" s="70"/>
       <c r="H30" s="70"/>
@@ -10280,7 +10264,7 @@
         <v>15</v>
       </c>
       <c r="N30" s="108" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O30" s="108" t="s">
         <v>6</v>
@@ -10298,19 +10282,19 @@
         <v>99</v>
       </c>
       <c r="AF30" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AJ30" s="30" t="s">
         <v>14</v>
       </c>
       <c r="AK30" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AL30" s="30" t="s">
         <v>6</v>
       </c>
       <c r="CE30" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="CO30" s="1" t="s">
         <v>115</v>
@@ -10326,7 +10310,7 @@
         <v>15</v>
       </c>
       <c r="R31" s="107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S31" s="107" t="s">
         <v>6</v>
@@ -10335,13 +10319,13 @@
         <v>82</v>
       </c>
       <c r="AB31" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AJ31" s="30" t="s">
         <v>14</v>
       </c>
       <c r="AK31" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AL31" s="30" t="s">
         <v>6</v>
@@ -10349,16 +10333,16 @@
     </row>
     <row r="32" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q32" s="107" t="s">
         <v>15</v>
       </c>
       <c r="R32" s="107" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="S32" s="107" t="s">
         <v>6</v>
@@ -10367,7 +10351,7 @@
         <v>83</v>
       </c>
       <c r="AB32" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AF32" s="1" t="s">
         <v>99</v>
@@ -10376,7 +10360,7 @@
         <v>14</v>
       </c>
       <c r="AK32" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AL32" s="30" t="s">
         <v>6</v>
@@ -10390,7 +10374,7 @@
         <v>15</v>
       </c>
       <c r="R33" s="107" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S33" s="107" t="s">
         <v>6</v>
@@ -10402,7 +10386,7 @@
         <v>14</v>
       </c>
       <c r="AK33" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AL33" s="34" t="s">
         <v>6</v>
@@ -10410,16 +10394,16 @@
     </row>
     <row r="34" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q34" s="108" t="s">
         <v>15</v>
       </c>
       <c r="R34" s="108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="S34" s="108" t="s">
         <v>6</v>
@@ -10441,16 +10425,16 @@
         <v>24</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AF36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="AJ36" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10458,7 +10442,7 @@
         <v>25</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF37" s="1" t="s">
         <v>79</v>
@@ -10466,21 +10450,21 @@
     </row>
     <row r="38" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AJ38" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D39" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="BT39" s="95" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="4:72" x14ac:dyDescent="0.2">
@@ -10490,7 +10474,7 @@
     </row>
     <row r="41" spans="4:72" x14ac:dyDescent="0.2">
       <c r="M41" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AJ41" s="1" t="s">
         <v>82</v>
@@ -10503,7 +10487,7 @@
     </row>
     <row r="43" spans="4:72" x14ac:dyDescent="0.2">
       <c r="M43" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="4:72" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Coming back from Denmark
</commit_message>
<xml_diff>
--- a/Example_dataset/Dataset_example_worksheet.xlsx
+++ b/Example_dataset/Dataset_example_worksheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/y.holtz/Dropbox/data_to_viz/Example_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yan/Dropbox/data_to_viz/Example_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2000" windowWidth="31840" windowHeight="17620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25220" windowHeight="14160" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SHENFA" sheetId="9" r:id="rId1"/>
@@ -24,9 +24,6 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -653,9 +650,6 @@
   </si>
   <si>
     <t>grouped barplot</t>
-  </si>
-  <si>
-    <t>Gene expression</t>
   </si>
   <si>
     <t>Story1Num2catSubgroup1value</t>
@@ -1046,10 +1040,13 @@
     <t>Perception of probability</t>
   </si>
   <si>
-    <t>bike / temperature ?</t>
-  </si>
-  <si>
     <t>Twitter connection of #rstat</t>
+  </si>
+  <si>
+    <t>House kaggle</t>
+  </si>
+  <si>
+    <t>Migration flow</t>
   </si>
 </sst>
 </file>
@@ -1947,18 +1944,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2036,6 +2021,52 @@
     </xf>
     <xf numFmtId="0" fontId="41" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="10"/>
@@ -2046,51 +2077,17 @@
     <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
@@ -2100,10 +2097,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3849,7 +3846,7 @@
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.2">
@@ -3859,12 +3856,12 @@
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D16" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3876,7 +3873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AY69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -3928,7 +3925,7 @@
       <c r="K9" s="54"/>
       <c r="L9" s="54"/>
       <c r="O9" s="73" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P9" s="54"/>
       <c r="Q9" s="54"/>
@@ -3952,7 +3949,7 @@
       <c r="AI9" s="54"/>
       <c r="AJ9" s="68"/>
       <c r="AL9" s="73" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AM9" s="54"/>
       <c r="AN9" s="54"/>
@@ -4035,22 +4032,22 @@
     </row>
     <row r="16" spans="3:51" ht="26" x14ac:dyDescent="0.3">
       <c r="O16" s="53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P16" s="54"/>
       <c r="Q16" s="54"/>
       <c r="S16" s="53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="T16" s="54"/>
       <c r="U16" s="54"/>
       <c r="W16" s="53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X16" s="54"/>
       <c r="Y16" s="54"/>
       <c r="AA16" s="53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AB16" s="54"/>
       <c r="AC16" s="54"/>
@@ -4074,48 +4071,48 @@
       <c r="J17" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="AL17" s="127" t="s">
+      <c r="AL17" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="AM17" s="127" t="s">
+      <c r="AM17" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="AN17" s="127" t="s">
+      <c r="AN17" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="AO17" s="127" t="s">
-        <v>287</v>
-      </c>
-      <c r="AQ17" s="127" t="s">
+      <c r="AO17" s="123" t="s">
+        <v>286</v>
+      </c>
+      <c r="AQ17" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="AR17" s="127" t="s">
+      <c r="AR17" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="AS17" s="127" t="s">
+      <c r="AS17" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="AT17" s="127" t="s">
-        <v>287</v>
-      </c>
-      <c r="AV17" s="127" t="s">
+      <c r="AT17" s="123" t="s">
+        <v>286</v>
+      </c>
+      <c r="AV17" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="AW17" s="146" t="s">
+      <c r="AW17" s="139" t="s">
         <v>95</v>
       </c>
-      <c r="AX17" s="127" t="s">
+      <c r="AX17" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="AY17" s="127" t="s">
-        <v>287</v>
+      <c r="AY17" s="123" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="3:51" x14ac:dyDescent="0.2">
       <c r="C18" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="119">
+      <c r="D18" s="115">
         <v>0.25</v>
       </c>
       <c r="F18" s="45" t="s">
@@ -4140,7 +4137,7 @@
         <v>7</v>
       </c>
       <c r="AO18" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AQ18" s="48" t="s">
         <v>13</v>
@@ -4152,7 +4149,7 @@
         <v>7</v>
       </c>
       <c r="AT18" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AV18" s="48" t="s">
         <v>13</v>
@@ -4164,14 +4161,14 @@
         <v>7</v>
       </c>
       <c r="AY18" s="46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="3:51" x14ac:dyDescent="0.2">
       <c r="C19" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="120">
+      <c r="D19" s="116">
         <v>0.3</v>
       </c>
       <c r="E19" s="33" t="s">
@@ -4199,7 +4196,7 @@
         <v>8</v>
       </c>
       <c r="AO19" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AQ19" s="48" t="s">
         <v>13</v>
@@ -4211,9 +4208,9 @@
         <v>8</v>
       </c>
       <c r="AT19" s="36" t="s">
-        <v>287</v>
-      </c>
-      <c r="AV19" s="117" t="s">
+        <v>286</v>
+      </c>
+      <c r="AV19" s="113" t="s">
         <v>14</v>
       </c>
       <c r="AW19" s="36">
@@ -4223,14 +4220,14 @@
         <v>11</v>
       </c>
       <c r="AY19" s="46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="3:51" x14ac:dyDescent="0.2">
       <c r="C20" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="120">
+      <c r="D20" s="116">
         <v>0.4</v>
       </c>
       <c r="F20" s="46" t="s">
@@ -4255,7 +4252,7 @@
         <v>9</v>
       </c>
       <c r="AO20" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AQ20" s="48" t="s">
         <v>13</v>
@@ -4267,9 +4264,9 @@
         <v>9</v>
       </c>
       <c r="AT20" s="36" t="s">
-        <v>287</v>
-      </c>
-      <c r="AV20" s="118" t="s">
+        <v>286</v>
+      </c>
+      <c r="AV20" s="114" t="s">
         <v>15</v>
       </c>
       <c r="AW20" s="36">
@@ -4279,75 +4276,75 @@
         <v>98</v>
       </c>
       <c r="AY20" s="46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="3:51" x14ac:dyDescent="0.2">
       <c r="C21" s="47" t="s">
-        <v>287</v>
-      </c>
-      <c r="D21" s="121" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="D21" s="117" t="s">
+        <v>286</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>287</v>
-      </c>
-      <c r="I21" s="117" t="s">
+        <v>286</v>
+      </c>
+      <c r="I21" s="113" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O21" s="127" t="s">
+      <c r="O21" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="P21" s="127" t="s">
+      <c r="P21" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="Q21" s="127" t="s">
+      <c r="Q21" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="S21" s="127" t="s">
+      <c r="S21" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="T21" s="127" t="s">
+      <c r="T21" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="U21" s="127" t="s">
+      <c r="U21" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="W21" s="127" t="s">
+      <c r="W21" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="X21" s="127" t="s">
+      <c r="X21" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="Y21" s="127" t="s">
+      <c r="Y21" s="123" t="s">
         <v>95</v>
       </c>
       <c r="Z21" s="70"/>
-      <c r="AA21" s="127" t="s">
+      <c r="AA21" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="AB21" s="127" t="s">
+      <c r="AB21" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="AC21" s="127" t="s">
+      <c r="AC21" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="AE21" s="127" t="s">
+      <c r="AE21" s="123" t="s">
+        <v>291</v>
+      </c>
+      <c r="AF21" s="123" t="s">
         <v>292</v>
       </c>
-      <c r="AF21" s="127" t="s">
-        <v>293</v>
-      </c>
-      <c r="AG21" s="127" t="s">
+      <c r="AG21" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="AL21" s="117" t="s">
+      <c r="AL21" s="113" t="s">
         <v>14</v>
       </c>
       <c r="AM21" s="46" t="s">
@@ -4357,9 +4354,9 @@
         <v>10</v>
       </c>
       <c r="AO21" s="36" t="s">
-        <v>287</v>
-      </c>
-      <c r="AQ21" s="117" t="s">
+        <v>286</v>
+      </c>
+      <c r="AQ21" s="113" t="s">
         <v>14</v>
       </c>
       <c r="AR21" s="6">
@@ -4369,23 +4366,23 @@
         <v>10</v>
       </c>
       <c r="AT21" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AV21" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AW21" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AX21" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AY21" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="3:51" x14ac:dyDescent="0.2">
-      <c r="I22" s="117" t="s">
+      <c r="I22" s="113" t="s">
         <v>14</v>
       </c>
       <c r="J22" s="6" t="s">
@@ -4414,7 +4411,7 @@
         <v>13</v>
       </c>
       <c r="X22" s="51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Y22" s="78" t="s">
         <v>2</v>
@@ -4424,7 +4421,7 @@
         <v>13</v>
       </c>
       <c r="AB22" s="51" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AC22" s="45" t="s">
         <v>2</v>
@@ -4432,13 +4429,13 @@
       <c r="AE22" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AF22" s="139" t="s">
+      <c r="AF22" s="135" t="s">
         <v>14</v>
       </c>
       <c r="AG22" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AL22" s="117" t="s">
+      <c r="AL22" s="113" t="s">
         <v>14</v>
       </c>
       <c r="AM22" s="46" t="s">
@@ -4448,9 +4445,9 @@
         <v>10</v>
       </c>
       <c r="AO22" s="36" t="s">
-        <v>287</v>
-      </c>
-      <c r="AQ22" s="117" t="s">
+        <v>286</v>
+      </c>
+      <c r="AQ22" s="113" t="s">
         <v>14</v>
       </c>
       <c r="AR22" s="46">
@@ -4460,21 +4457,21 @@
         <v>10</v>
       </c>
       <c r="AT22" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="3:51" x14ac:dyDescent="0.2">
       <c r="I23" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O23" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="P23" s="125" t="s">
-        <v>255</v>
+      <c r="P23" s="121" t="s">
+        <v>254</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>4</v>
@@ -4493,7 +4490,7 @@
         <v>13</v>
       </c>
       <c r="X23" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Y23" s="3" t="s">
         <v>4</v>
@@ -4503,7 +4500,7 @@
         <v>13</v>
       </c>
       <c r="AB23" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AC23" s="46" t="s">
         <v>3</v>
@@ -4511,35 +4508,35 @@
       <c r="AE23" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AF23" s="140" t="s">
+      <c r="AF23" s="136" t="s">
         <v>15</v>
       </c>
       <c r="AG23" s="36" t="s">
         <v>2</v>
       </c>
       <c r="AL23" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AM23" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AN23" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AO23" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AQ23" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AR23" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AS23" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AT23" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AV23" s="1" t="s">
         <v>126</v>
@@ -4549,7 +4546,7 @@
       <c r="D24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O24" s="126" t="s">
+      <c r="O24" s="122" t="s">
         <v>14</v>
       </c>
       <c r="P24" s="46" t="s">
@@ -4562,17 +4559,17 @@
       <c r="S24" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="T24" s="125" t="s">
-        <v>255</v>
+      <c r="T24" s="121" t="s">
+        <v>254</v>
       </c>
       <c r="U24" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="W24" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="X24" s="117" t="s">
-        <v>290</v>
+      <c r="W24" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="X24" s="113" t="s">
+        <v>289</v>
       </c>
       <c r="Y24" s="3" t="s">
         <v>5</v>
@@ -4581,16 +4578,16 @@
       <c r="AA24" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="AB24" s="138" t="s">
-        <v>289</v>
+      <c r="AB24" s="134" t="s">
+        <v>288</v>
       </c>
       <c r="AC24" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="AE24" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF24" s="141" t="s">
+      <c r="AE24" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF24" s="137" t="s">
         <v>13</v>
       </c>
       <c r="AG24" s="36" t="s">
@@ -4601,17 +4598,17 @@
       <c r="D25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O25" s="126" t="s">
-        <v>14</v>
-      </c>
-      <c r="P25" s="125" t="s">
-        <v>255</v>
+      <c r="O25" s="122" t="s">
+        <v>14</v>
+      </c>
+      <c r="P25" s="121" t="s">
+        <v>254</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R25" s="70"/>
-      <c r="S25" s="117" t="s">
+      <c r="S25" s="113" t="s">
         <v>14</v>
       </c>
       <c r="T25" s="46" t="s">
@@ -4620,29 +4617,29 @@
       <c r="U25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="W25" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="X25" s="117" t="s">
-        <v>291</v>
+      <c r="W25" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="X25" s="113" t="s">
+        <v>290</v>
       </c>
       <c r="Y25" s="3">
         <v>3.2</v>
       </c>
       <c r="Z25" s="70"/>
-      <c r="AA25" s="132" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="131" t="s">
-        <v>289</v>
-      </c>
-      <c r="AC25" s="136" t="s">
+      <c r="AA25" s="128" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB25" s="127" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC25" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="AE25" s="122" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF25" s="142" t="s">
+      <c r="AE25" s="118" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF25" s="138" t="s">
         <v>15</v>
       </c>
       <c r="AG25" s="37" t="s">
@@ -4662,16 +4659,16 @@
       <c r="I26" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="O26" s="128" t="s">
-        <v>287</v>
+      <c r="O26" s="124" t="s">
+        <v>286</v>
       </c>
       <c r="P26" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Q26" s="37" t="s">
-        <v>287</v>
-      </c>
-      <c r="S26" s="117" t="s">
+        <v>286</v>
+      </c>
+      <c r="S26" s="113" t="s">
         <v>14</v>
       </c>
       <c r="T26" s="46" t="s">
@@ -4681,19 +4678,19 @@
         <v>6</v>
       </c>
       <c r="W26" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="X26" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Y26" s="37" t="s">
-        <v>287</v>
-      </c>
-      <c r="AA26" s="117" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA26" s="113" t="s">
         <v>14</v>
       </c>
       <c r="AB26" s="49" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AC26" s="46" t="s">
         <v>5</v>
@@ -4708,7 +4705,7 @@
         <v>140</v>
       </c>
       <c r="AR26" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AV26" s="1" t="s">
         <v>109</v>
@@ -4727,28 +4724,28 @@
       <c r="J27" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="S27" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="T27" s="125" t="s">
-        <v>255</v>
+      <c r="S27" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="T27" s="121" t="s">
+        <v>254</v>
       </c>
       <c r="U27" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="AA27" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB27" s="133" t="s">
-        <v>290</v>
+      <c r="AA27" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB27" s="129" t="s">
+        <v>289</v>
       </c>
       <c r="AC27" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="AE27" s="145" t="s">
-        <v>295</v>
-      </c>
-      <c r="AF27" s="145"/>
+      <c r="AE27" s="157" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF27" s="157"/>
       <c r="AL27" s="58" t="s">
         <v>121</v>
       </c>
@@ -4764,34 +4761,34 @@
         <v>89</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>287</v>
-      </c>
-      <c r="AA28" s="117" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA28" s="113" t="s">
         <v>14</v>
       </c>
       <c r="AB28" s="49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AC28" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="AD28" s="143" t="s">
-        <v>294</v>
-      </c>
-      <c r="AE28" s="144"/>
-      <c r="AF28" s="127" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG28" s="127" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH28" s="127" t="s">
+      <c r="AD28" s="155" t="s">
+        <v>293</v>
+      </c>
+      <c r="AE28" s="156"/>
+      <c r="AF28" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG28" s="123" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH28" s="123" t="s">
         <v>15</v>
       </c>
       <c r="AQ28" s="1" t="s">
@@ -4813,16 +4810,16 @@
       </c>
       <c r="R29" s="58"/>
       <c r="U29" s="58"/>
-      <c r="AA29" s="122" t="s">
+      <c r="AA29" s="118" t="s">
         <v>14</v>
       </c>
       <c r="AB29" s="50" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AC29" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="AE29" s="127" t="s">
+      <c r="AE29" s="123" t="s">
         <v>13</v>
       </c>
       <c r="AF29" s="45" t="s">
@@ -4835,10 +4832,10 @@
         <v>1.3</v>
       </c>
       <c r="AL29" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AM29" s="95" t="s">
         <v>243</v>
-      </c>
-      <c r="AM29" s="95" t="s">
-        <v>244</v>
       </c>
       <c r="AQ29" s="1" t="s">
         <v>118</v>
@@ -4854,7 +4851,7 @@
       <c r="J30" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="AE30" s="127" t="s">
+      <c r="AE30" s="123" t="s">
         <v>14</v>
       </c>
       <c r="AF30" s="46">
@@ -4886,7 +4883,7 @@
       <c r="S31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AE31" s="127" t="s">
+      <c r="AE31" s="123" t="s">
         <v>15</v>
       </c>
       <c r="AF31" s="47" t="s">
@@ -4899,7 +4896,7 @@
         <v>32</v>
       </c>
       <c r="AL31" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AV31" s="1" t="s">
         <v>104</v>
@@ -4919,10 +4916,10 @@
         <v>88</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AL32" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AV32" s="1" t="s">
         <v>105</v>
@@ -4937,7 +4934,7 @@
         <v>78</v>
       </c>
       <c r="AA33" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE33" s="1" t="s">
         <v>163</v>
@@ -4949,19 +4946,19 @@
         <v>24</v>
       </c>
       <c r="AA34" s="58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AE34" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AL34" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AN34" s="58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AV34" s="68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="4:48" x14ac:dyDescent="0.2">
@@ -4969,13 +4966,13 @@
         <v>25</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AE35" s="1" t="s">
         <v>173</v>
       </c>
       <c r="AL35" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AV35" s="68"/>
     </row>
@@ -4990,10 +4987,10 @@
         <v>99</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AF37" s="76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AG37" s="95"/>
     </row>
@@ -5015,7 +5012,7 @@
     </row>
     <row r="40" spans="4:48" x14ac:dyDescent="0.2">
       <c r="O40" s="68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P40" s="68"/>
       <c r="Q40" s="68"/>
@@ -5146,22 +5143,22 @@
         <v>204</v>
       </c>
       <c r="O46" s="90" t="s">
+        <v>206</v>
+      </c>
+      <c r="S46" s="90" t="s">
         <v>207</v>
       </c>
-      <c r="S46" s="90" t="s">
-        <v>208</v>
-      </c>
       <c r="W46" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA46" s="90" t="s">
+        <v>330</v>
+      </c>
+      <c r="AE46" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="AA46" s="90" t="s">
-        <v>331</v>
-      </c>
-      <c r="AE46" s="90" t="s">
-        <v>215</v>
-      </c>
       <c r="AH46" s="90" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AL46" s="90"/>
       <c r="AM46" s="70"/>
@@ -5169,28 +5166,28 @@
         <v>201</v>
       </c>
       <c r="AV46" s="90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="4:48" x14ac:dyDescent="0.2">
       <c r="D47" s="90" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I47" s="90" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O47" s="90"/>
       <c r="S47" s="90" t="s">
         <v>54</v>
       </c>
       <c r="W47" s="90" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AA47" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="AE47" s="161" t="s">
-        <v>301</v>
+      <c r="AE47" s="154" t="s">
+        <v>300</v>
       </c>
       <c r="AL47" s="90"/>
       <c r="AM47" s="70"/>
@@ -5200,11 +5197,11 @@
       <c r="AV47" s="90"/>
     </row>
     <row r="48" spans="4:48" x14ac:dyDescent="0.2">
-      <c r="AE48" s="161" t="s">
+      <c r="AE48" s="154" t="s">
+        <v>301</v>
+      </c>
+      <c r="AH48" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="AH48" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="AM48" s="70"/>
     </row>
@@ -5212,19 +5209,19 @@
       <c r="AM49" s="70"/>
     </row>
     <row r="50" spans="26:39" x14ac:dyDescent="0.2">
-      <c r="AE50" s="161" t="s">
+      <c r="AE50" s="154" t="s">
+        <v>303</v>
+      </c>
+      <c r="AM50" s="70"/>
+    </row>
+    <row r="51" spans="26:39" x14ac:dyDescent="0.2">
+      <c r="AE51" s="154" t="s">
         <v>304</v>
-      </c>
-      <c r="AM50" s="70"/>
-    </row>
-    <row r="51" spans="26:39" x14ac:dyDescent="0.2">
-      <c r="AE51" s="161" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="53" spans="26:39" x14ac:dyDescent="0.2">
       <c r="AH53" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="61" spans="26:39" x14ac:dyDescent="0.2">
@@ -5294,8 +5291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AN43"/>
   <sheetViews>
-    <sheetView topLeftCell="Q5" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="AI43" sqref="AI43"/>
+    <sheetView topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5317,14 +5314,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:39" ht="62" x14ac:dyDescent="0.7">
-      <c r="K3" s="113" t="s">
+      <c r="K3" s="158" t="s">
         <v>130</v>
       </c>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="115"/>
+      <c r="L3" s="159"/>
+      <c r="M3" s="159"/>
+      <c r="N3" s="159"/>
+      <c r="O3" s="159"/>
+      <c r="P3" s="160"/>
     </row>
     <row r="9" spans="3:39" ht="26" x14ac:dyDescent="0.3">
       <c r="C9" s="59" t="s">
@@ -5460,7 +5457,7 @@
         <v>144</v>
       </c>
       <c r="AG15" s="111" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AI15" s="111" t="s">
         <v>95</v>
@@ -5475,7 +5472,7 @@
         <v>144</v>
       </c>
       <c r="AM15" s="111" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="3:39" x14ac:dyDescent="0.2">
@@ -5525,7 +5522,7 @@
         <v>7</v>
       </c>
       <c r="AG16" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AI16" s="6" t="s">
         <v>2</v>
@@ -5540,7 +5537,7 @@
         <v>7</v>
       </c>
       <c r="AM16" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="3:40" x14ac:dyDescent="0.2">
@@ -5590,7 +5587,7 @@
         <v>8</v>
       </c>
       <c r="AG17" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AI17" s="6" t="s">
         <v>3</v>
@@ -5605,7 +5602,7 @@
         <v>8</v>
       </c>
       <c r="AM17" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="3:40" x14ac:dyDescent="0.2">
@@ -5655,7 +5652,7 @@
         <v>9</v>
       </c>
       <c r="AG18" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AI18" s="6" t="s">
         <v>4</v>
@@ -5670,7 +5667,7 @@
         <v>9</v>
       </c>
       <c r="AM18" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="3:40" x14ac:dyDescent="0.2">
@@ -5720,7 +5717,7 @@
         <v>10</v>
       </c>
       <c r="AG19" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AI19" s="6" t="s">
         <v>5</v>
@@ -5735,77 +5732,77 @@
         <v>10</v>
       </c>
       <c r="AM19" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Q20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="V20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="W20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Y20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Z20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AA20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AC20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AD20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AE20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AF20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AG20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AI20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AJ20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AK20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AL20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AM20" s="112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="3:40" x14ac:dyDescent="0.2">
       <c r="H21" s="89" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I21" s="89"/>
       <c r="J21" s="89"/>
@@ -5899,7 +5896,7 @@
         <v>142</v>
       </c>
       <c r="AI29" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="3:40" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5956,7 +5953,7 @@
     </row>
     <row r="37" spans="3:40" x14ac:dyDescent="0.2">
       <c r="AB37" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AN37" s="88"/>
     </row>
@@ -6004,7 +6001,7 @@
     </row>
     <row r="42" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C42" s="90" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I42" s="90" t="s">
         <v>333</v>
@@ -6015,27 +6012,27 @@
       </c>
       <c r="Q42" s="90"/>
       <c r="U42" s="90" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB42" s="90" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI42" s="90" t="s">
         <v>217</v>
-      </c>
-      <c r="AB42" s="90" t="s">
-        <v>284</v>
-      </c>
-      <c r="AI42" s="90" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="43" spans="3:40" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AB43" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -6054,8 +6051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:T156"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14:S21"/>
+    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6070,14 +6067,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:20" ht="62" x14ac:dyDescent="0.7">
-      <c r="L3" s="113" t="s">
+      <c r="L3" s="158" t="s">
         <v>148</v>
       </c>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="115"/>
+      <c r="M3" s="159"/>
+      <c r="N3" s="159"/>
+      <c r="O3" s="159"/>
+      <c r="P3" s="159"/>
+      <c r="Q3" s="160"/>
     </row>
     <row r="9" spans="3:20" ht="26" x14ac:dyDescent="0.3">
       <c r="C9" s="59" t="s">
@@ -6086,7 +6083,7 @@
       <c r="D9" s="59"/>
       <c r="E9" s="54"/>
       <c r="H9" s="73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I9" s="59"/>
       <c r="J9" s="54"/>
@@ -6138,10 +6135,10 @@
         <v>13</v>
       </c>
       <c r="H14" s="111" t="s">
+        <v>218</v>
+      </c>
+      <c r="J14" s="111" t="s">
         <v>219</v>
-      </c>
-      <c r="J14" s="111" t="s">
-        <v>220</v>
       </c>
       <c r="L14" s="111" t="s">
         <v>95</v>
@@ -6175,7 +6172,7 @@
       <c r="L15" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="M15" s="141" t="s">
+      <c r="M15" s="137" t="s">
         <v>150</v>
       </c>
       <c r="O15" s="51" t="s">
@@ -6204,7 +6201,7 @@
       <c r="L16" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="141" t="s">
+      <c r="M16" s="137" t="s">
         <v>150</v>
       </c>
       <c r="O16" s="48" t="s">
@@ -6216,7 +6213,7 @@
       <c r="R16" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="S16" s="118" t="s">
+      <c r="S16" s="114" t="s">
         <v>15</v>
       </c>
     </row>
@@ -6233,7 +6230,7 @@
       <c r="L17" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="M17" s="147" t="s">
+      <c r="M17" s="140" t="s">
         <v>151</v>
       </c>
       <c r="O17" s="48" t="s">
@@ -6245,13 +6242,13 @@
       <c r="R17" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="S17" s="117" t="s">
+      <c r="S17" s="113" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C18" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>154</v>
@@ -6259,19 +6256,19 @@
       <c r="J18" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="L18" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="M18" s="148" t="s">
+      <c r="L18" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="O18" s="117" t="s">
+      <c r="O18" s="113" t="s">
         <v>14</v>
       </c>
       <c r="P18" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="R18" s="117" t="s">
+      <c r="R18" s="113" t="s">
         <v>14</v>
       </c>
       <c r="S18" s="48" t="s">
@@ -6280,24 +6277,24 @@
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.2">
       <c r="H19" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="L19" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="M19" s="148" t="s">
+        <v>286</v>
+      </c>
+      <c r="L19" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="141" t="s">
         <v>152</v>
       </c>
-      <c r="O19" s="117" t="s">
+      <c r="O19" s="113" t="s">
         <v>14</v>
       </c>
       <c r="P19" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="R19" s="117" t="s">
+      <c r="R19" s="113" t="s">
         <v>14</v>
       </c>
       <c r="S19" s="48" t="s">
@@ -6309,22 +6306,22 @@
         <v>191</v>
       </c>
       <c r="L20" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M20" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O20" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P20" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R20" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S20" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.2">
@@ -6408,7 +6405,7 @@
         <v>80</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>25</v>
@@ -6439,7 +6436,7 @@
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O34" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
@@ -6464,33 +6461,33 @@
         <v>203</v>
       </c>
       <c r="H40" s="90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L40" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="O40" s="90" t="s">
+        <v>206</v>
+      </c>
+      <c r="R40" s="90" t="s">
         <v>214</v>
-      </c>
-      <c r="O40" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="R40" s="90" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C41" s="90" t="s">
+        <v>326</v>
+      </c>
+      <c r="H41" s="90" t="s">
         <v>327</v>
-      </c>
-      <c r="H41" s="90" t="s">
-        <v>328</v>
       </c>
       <c r="L41" s="90" t="s">
         <v>54</v>
       </c>
       <c r="O41" s="90" t="s">
-        <v>206</v>
+        <v>54</v>
       </c>
       <c r="R41" s="90" t="s">
-        <v>54</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.2">
@@ -7210,24 +7207,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:30" ht="62" x14ac:dyDescent="0.7">
-      <c r="H3" s="113" t="s">
-        <v>297</v>
-      </c>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="115"/>
+      <c r="H3" s="158" t="s">
+        <v>296</v>
+      </c>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
+      <c r="L3" s="159"/>
+      <c r="M3" s="160"/>
     </row>
     <row r="4" spans="3:30" x14ac:dyDescent="0.2">
-      <c r="H4" s="116" t="s">
+      <c r="H4" s="161" t="s">
         <v>164</v>
       </c>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
-      <c r="M4" s="116"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
+      <c r="L4" s="161"/>
+      <c r="M4" s="161"/>
     </row>
     <row r="8" spans="3:30" x14ac:dyDescent="0.2">
       <c r="L8" s="68"/>
@@ -7261,7 +7258,7 @@
       <c r="H9" s="54"/>
       <c r="I9" s="54"/>
       <c r="L9" s="94" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M9" s="59"/>
       <c r="N9" s="54"/>
@@ -7302,7 +7299,7 @@
       <c r="S12" s="54"/>
       <c r="T12" s="54"/>
       <c r="V12" s="74" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="W12" s="54"/>
       <c r="X12" s="54"/>
@@ -7315,19 +7312,19 @@
       <c r="AD12" s="54"/>
     </row>
     <row r="13" spans="3:30" x14ac:dyDescent="0.2">
-      <c r="C13" s="127" t="s">
+      <c r="C13" s="123" t="s">
+        <v>291</v>
+      </c>
+      <c r="D13" s="123" t="s">
         <v>292</v>
       </c>
-      <c r="D13" s="127" t="s">
-        <v>293</v>
-      </c>
-      <c r="E13" s="127" t="s">
+      <c r="E13" s="123" t="s">
         <v>95</v>
       </c>
       <c r="H13" s="111" t="s">
         <v>171</v>
       </c>
-      <c r="I13" s="127" t="s">
+      <c r="I13" s="123" t="s">
         <v>129</v>
       </c>
     </row>
@@ -7335,7 +7332,7 @@
       <c r="C14" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="139" t="s">
+      <c r="D14" s="135" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="35" t="s">
@@ -7370,7 +7367,7 @@
       <c r="C15" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="140" t="s">
+      <c r="D15" s="136" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="36" t="s">
@@ -7379,57 +7376,57 @@
       <c r="F15" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="117" t="s">
+      <c r="H15" s="113" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="46">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L15" s="127" t="s">
+      <c r="L15" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="M15" s="127" t="s">
+      <c r="M15" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="127" t="s">
+      <c r="P15" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="Q15" s="127" t="s">
+      <c r="Q15" s="123" t="s">
         <v>67</v>
       </c>
       <c r="S15" s="111" t="s">
         <v>171</v>
       </c>
-      <c r="T15" s="127" t="s">
-        <v>298</v>
-      </c>
-      <c r="V15" s="127" t="s">
+      <c r="T15" s="123" t="s">
+        <v>297</v>
+      </c>
+      <c r="V15" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="W15" s="127" t="s">
+      <c r="W15" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="X15" s="127" t="s">
+      <c r="X15" s="123" t="s">
         <v>129</v>
       </c>
-      <c r="Z15" s="127" t="s">
+      <c r="Z15" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="AA15" s="127" t="s">
+      <c r="AA15" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="AC15" s="127" t="s">
+      <c r="AC15" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="AD15" s="127" t="s">
+      <c r="AD15" s="123" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="3:30" x14ac:dyDescent="0.2">
-      <c r="C16" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="141" t="s">
+      <c r="C16" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="137" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="36" t="s">
@@ -7438,7 +7435,7 @@
       <c r="F16" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="H16" s="149" t="s">
+      <c r="H16" s="142" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="47">
@@ -7456,7 +7453,7 @@
       <c r="Q16" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="S16" s="155" t="s">
+      <c r="S16" s="148" t="s">
         <v>27</v>
       </c>
       <c r="T16" s="45">
@@ -7477,18 +7474,18 @@
       <c r="AA16" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AC16" s="158" t="s">
+      <c r="AC16" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="AD16" s="137" t="s">
+      <c r="AD16" s="133" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C17" s="122" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="142" t="s">
+      <c r="C17" s="118" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="138" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="37" t="s">
@@ -7497,16 +7494,16 @@
       <c r="L17" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="M17" s="117" t="s">
+      <c r="M17" s="113" t="s">
         <v>14</v>
       </c>
       <c r="P17" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="Q17" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="S17" s="156" t="s">
+      <c r="Q17" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="S17" s="149" t="s">
         <v>28</v>
       </c>
       <c r="T17" s="46">
@@ -7515,7 +7512,7 @@
       <c r="V17" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="W17" s="117" t="s">
+      <c r="W17" s="113" t="s">
         <v>14</v>
       </c>
       <c r="X17" s="46">
@@ -7524,10 +7521,10 @@
       <c r="Z17" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="AA17" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC17" s="151" t="s">
+      <c r="AA17" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC17" s="144" t="s">
         <v>30</v>
       </c>
       <c r="AD17" s="49" t="s">
@@ -7535,21 +7532,21 @@
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C18" s="150" t="s">
-        <v>296</v>
-      </c>
-      <c r="D18" s="150"/>
-      <c r="E18" s="150"/>
+      <c r="C18" s="143" t="s">
+        <v>295</v>
+      </c>
+      <c r="D18" s="143"/>
+      <c r="E18" s="143"/>
       <c r="L18" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="M18" s="155" t="s">
+      <c r="M18" s="148" t="s">
         <v>27</v>
       </c>
       <c r="P18" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" s="155" t="s">
+      <c r="Q18" s="148" t="s">
         <v>27</v>
       </c>
       <c r="R18" s="33" t="s">
@@ -7564,7 +7561,7 @@
       <c r="V18" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="W18" s="155" t="s">
+      <c r="W18" s="148" t="s">
         <v>27</v>
       </c>
       <c r="X18" s="46">
@@ -7573,16 +7570,16 @@
       <c r="Z18" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AA18" s="155" t="s">
+      <c r="AA18" s="148" t="s">
         <v>27</v>
       </c>
       <c r="AB18" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="AC18" s="159" t="s">
+      <c r="AC18" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="AD18" s="160" t="s">
+      <c r="AD18" s="153" t="s">
         <v>28</v>
       </c>
     </row>
@@ -7593,16 +7590,16 @@
       <c r="L19" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="156" t="s">
+      <c r="M19" s="149" t="s">
         <v>28</v>
       </c>
       <c r="P19" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="Q19" s="156" t="s">
+      <c r="Q19" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="S19" s="152" t="s">
+      <c r="S19" s="145" t="s">
         <v>30</v>
       </c>
       <c r="T19" s="47">
@@ -7611,7 +7608,7 @@
       <c r="V19" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="W19" s="156" t="s">
+      <c r="W19" s="149" t="s">
         <v>28</v>
       </c>
       <c r="X19" s="46">
@@ -7620,7 +7617,7 @@
       <c r="Z19" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AA19" s="156" t="s">
+      <c r="AA19" s="149" t="s">
         <v>28</v>
       </c>
     </row>
@@ -7658,26 +7655,26 @@
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C21" s="145" t="s">
-        <v>295</v>
-      </c>
-      <c r="D21" s="145"/>
+      <c r="C21" s="157" t="s">
+        <v>294</v>
+      </c>
+      <c r="D21" s="157"/>
       <c r="L21" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="151" t="s">
+      <c r="M21" s="144" t="s">
         <v>30</v>
       </c>
       <c r="P21" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="Q21" s="151" t="s">
+      <c r="Q21" s="144" t="s">
         <v>30</v>
       </c>
       <c r="V21" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="W21" s="151" t="s">
+      <c r="W21" s="144" t="s">
         <v>30</v>
       </c>
       <c r="X21" s="46">
@@ -7686,60 +7683,60 @@
       <c r="Z21" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="AA21" s="151" t="s">
+      <c r="AA21" s="144" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B22" s="162" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C22" s="163"/>
-      <c r="D22" s="127" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="127" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="127" t="s">
+      <c r="D22" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="123" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="123" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="111" t="s">
         <v>171</v>
       </c>
-      <c r="I22" s="127" t="s">
+      <c r="I22" s="123" t="s">
         <v>129</v>
       </c>
       <c r="L22" s="50" t="s">
-        <v>287</v>
-      </c>
-      <c r="M22" s="152" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="M22" s="145" t="s">
+        <v>286</v>
       </c>
       <c r="P22" s="50" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q22" s="152" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="Q22" s="145" t="s">
+        <v>286</v>
       </c>
       <c r="V22" s="50" t="s">
-        <v>287</v>
-      </c>
-      <c r="W22" s="152" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="W22" s="145" t="s">
+        <v>286</v>
       </c>
       <c r="X22" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Z22" s="50" t="s">
-        <v>287</v>
-      </c>
-      <c r="AA22" s="152" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="AA22" s="145" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C23" s="127" t="s">
+      <c r="C23" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -7765,7 +7762,7 @@
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C24" s="127" t="s">
+      <c r="C24" s="123" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="46">
@@ -7780,7 +7777,7 @@
       <c r="G24" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="117" t="s">
+      <c r="H24" s="113" t="s">
         <v>14</v>
       </c>
       <c r="I24" s="46">
@@ -7812,32 +7809,32 @@
       <c r="F25" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="149" t="s">
+      <c r="H25" s="142" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="47">
         <v>10</v>
       </c>
-      <c r="L25" s="127" t="s">
+      <c r="L25" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="M25" s="127" t="s">
+      <c r="M25" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="N25" s="127" t="s">
-        <v>287</v>
-      </c>
-      <c r="P25" s="127" t="s">
+      <c r="N25" s="123" t="s">
+        <v>286</v>
+      </c>
+      <c r="P25" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="Q25" s="127" t="s">
+      <c r="Q25" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="R25" s="127" t="s">
-        <v>287</v>
-      </c>
-      <c r="S25" s="127" t="s">
-        <v>298</v>
+      <c r="R25" s="123" t="s">
+        <v>286</v>
+      </c>
+      <c r="S25" s="123" t="s">
+        <v>297</v>
       </c>
       <c r="Z25" s="76"/>
     </row>
@@ -7845,20 +7842,20 @@
       <c r="L26" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="M26" s="123" t="s">
+      <c r="M26" s="119" t="s">
         <v>27</v>
       </c>
       <c r="N26" s="45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P26" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="Q26" s="123" t="s">
+      <c r="Q26" s="119" t="s">
         <v>27</v>
       </c>
       <c r="R26" s="45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S26" s="45" t="s">
         <v>2</v>
@@ -7871,20 +7868,20 @@
       <c r="L27" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="M27" s="153" t="s">
+      <c r="M27" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="N27" s="136" t="s">
-        <v>287</v>
+      <c r="N27" s="132" t="s">
+        <v>286</v>
       </c>
       <c r="P27" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="Q27" s="153" t="s">
+      <c r="Q27" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="R27" s="136" t="s">
-        <v>287</v>
+      <c r="R27" s="132" t="s">
+        <v>286</v>
       </c>
       <c r="S27" s="46" t="s">
         <v>3</v>
@@ -7894,20 +7891,20 @@
       <c r="L28" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="M28" s="124" t="s">
+      <c r="M28" s="120" t="s">
         <v>28</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P28" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="Q28" s="124" t="s">
+      <c r="Q28" s="120" t="s">
         <v>28</v>
       </c>
       <c r="R28" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S28" s="46" t="s">
         <v>4</v>
@@ -7917,25 +7914,25 @@
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="L29" s="131" t="s">
-        <v>13</v>
-      </c>
-      <c r="M29" s="154" t="s">
+      <c r="L29" s="127" t="s">
+        <v>13</v>
+      </c>
+      <c r="M29" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="N29" s="135" t="s">
-        <v>287</v>
-      </c>
-      <c r="P29" s="131" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q29" s="154" t="s">
+      <c r="N29" s="131" t="s">
+        <v>286</v>
+      </c>
+      <c r="P29" s="127" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q29" s="147" t="s">
         <v>28</v>
       </c>
-      <c r="R29" s="135" t="s">
-        <v>287</v>
-      </c>
-      <c r="S29" s="136" t="s">
+      <c r="R29" s="131" t="s">
+        <v>286</v>
+      </c>
+      <c r="S29" s="132" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7943,23 +7940,23 @@
       <c r="C30" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L30" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="M30" s="129" t="s">
+      <c r="L30" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="N30" s="157" t="s">
-        <v>287</v>
-      </c>
-      <c r="P30" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q30" s="129" t="s">
+      <c r="N30" s="150" t="s">
+        <v>286</v>
+      </c>
+      <c r="P30" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q30" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="R30" s="157" t="s">
-        <v>287</v>
+      <c r="R30" s="150" t="s">
+        <v>286</v>
       </c>
       <c r="S30" s="46" t="s">
         <v>5</v>
@@ -7969,23 +7966,23 @@
       <c r="C31" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L31" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="M31" s="133" t="s">
+      <c r="L31" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="N31" s="136" t="s">
-        <v>287</v>
-      </c>
-      <c r="P31" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q31" s="133" t="s">
+      <c r="N31" s="132" t="s">
+        <v>286</v>
+      </c>
+      <c r="P31" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q31" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="R31" s="136" t="s">
-        <v>287</v>
+      <c r="R31" s="132" t="s">
+        <v>286</v>
       </c>
       <c r="S31" s="46" t="s">
         <v>22</v>
@@ -7995,46 +7992,46 @@
       <c r="C32" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="L32" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="134" t="s">
+      <c r="L32" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="130" t="s">
         <v>30</v>
       </c>
       <c r="N32" s="36" t="s">
-        <v>287</v>
-      </c>
-      <c r="P32" s="117" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q32" s="134" t="s">
+        <v>286</v>
+      </c>
+      <c r="P32" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q32" s="130" t="s">
         <v>30</v>
       </c>
       <c r="R32" s="36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S32" s="46" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="3:26" x14ac:dyDescent="0.2">
-      <c r="L33" s="122" t="s">
-        <v>14</v>
-      </c>
-      <c r="M33" s="130" t="s">
+      <c r="L33" s="118" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="126" t="s">
         <v>30</v>
       </c>
       <c r="N33" s="37" t="s">
-        <v>287</v>
-      </c>
-      <c r="P33" s="122" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q33" s="130" t="s">
+        <v>286</v>
+      </c>
+      <c r="P33" s="118" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q33" s="126" t="s">
         <v>30</v>
       </c>
       <c r="R33" s="37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S33" s="47" t="s">
         <v>6</v>
@@ -8042,10 +8039,10 @@
     </row>
     <row r="34" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D34" s="76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E34" s="95"/>
       <c r="F34" s="95"/>
@@ -8064,7 +8061,7 @@
     </row>
     <row r="38" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q38" s="68"/>
     </row>
@@ -8095,7 +8092,7 @@
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.2">
       <c r="N43" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="3:26" x14ac:dyDescent="0.2">
@@ -8111,7 +8108,7 @@
     </row>
     <row r="45" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C45" s="90" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L45" s="75"/>
       <c r="M45" s="75"/>
@@ -8125,21 +8122,21 @@
       <c r="S45" s="75"/>
       <c r="T45" s="75"/>
       <c r="V45" s="90" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z45" s="90" t="s">
         <v>222</v>
-      </c>
-      <c r="Z45" s="90" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="46" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C46" s="90" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L46" s="68"/>
       <c r="M46" s="68"/>
       <c r="N46" s="68"/>
       <c r="O46" s="93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P46" s="68"/>
       <c r="Q46" s="68"/>
@@ -8155,10 +8152,10 @@
     </row>
     <row r="47" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O47" s="90" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -8191,38 +8188,38 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="123" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="123" t="s">
         <v>307</v>
       </c>
-      <c r="C6" s="127" t="s">
+      <c r="E6" s="123" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="123" t="s">
+        <v>307</v>
+      </c>
+      <c r="G6" s="123" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="123" t="s">
         <v>308</v>
       </c>
-      <c r="E6" s="127" t="s">
-        <v>307</v>
-      </c>
-      <c r="F6" s="127" t="s">
-        <v>308</v>
-      </c>
-      <c r="G6" s="127" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" s="127" t="s">
+      <c r="K6" s="123" t="s">
+        <v>311</v>
+      </c>
+      <c r="L6" s="123" t="s">
         <v>309</v>
       </c>
-      <c r="K6" s="127" t="s">
+      <c r="M6" s="123" t="s">
+        <v>310</v>
+      </c>
+      <c r="O6" s="123" t="s">
         <v>312</v>
       </c>
-      <c r="L6" s="127" t="s">
-        <v>310</v>
-      </c>
-      <c r="M6" s="127" t="s">
-        <v>311</v>
-      </c>
-      <c r="O6" s="127" t="s">
+      <c r="P6" s="123" t="s">
         <v>313</v>
-      </c>
-      <c r="P6" s="127" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
@@ -8254,7 +8251,7 @@
         <v>140</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P7" s="35">
         <v>23</v>
@@ -8289,7 +8286,7 @@
         <v>142.30000000000001</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P8" s="36">
         <v>12</v>
@@ -8324,7 +8321,7 @@
         <v>123.8</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P9" s="36">
         <v>9</v>
@@ -8359,7 +8356,7 @@
         <v>126</v>
       </c>
       <c r="O10" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P10" s="37">
         <v>10</v>
@@ -8372,27 +8369,27 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="91" t="s">
+        <v>319</v>
+      </c>
+      <c r="E19" s="91" t="s">
         <v>320</v>
-      </c>
-      <c r="E19" s="91" t="s">
-        <v>321</v>
       </c>
       <c r="J19" s="91">
         <v>19</v>
       </c>
       <c r="O19" s="90" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E20" s="90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J20" s="90" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O20" s="90" t="s">
         <v>54</v>
@@ -8411,20 +8408,20 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -8476,31 +8473,31 @@
     <row r="28" spans="1:1" s="54" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="75" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P44" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q45" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="26" x14ac:dyDescent="0.3">
       <c r="A46" s="82" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q47" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" s="75" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -8576,7 +8573,7 @@
       <c r="AW7" s="68"/>
       <c r="AX7" s="68"/>
       <c r="AZ7" s="73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="BA7" s="54"/>
       <c r="BB7" s="54"/>
@@ -8718,7 +8715,7 @@
       <c r="CK11" s="54"/>
       <c r="CL11" s="54"/>
       <c r="CO11" s="53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="CP11" s="54"/>
       <c r="CQ11" s="54"/>
@@ -8761,7 +8758,7 @@
         <v>96</v>
       </c>
       <c r="BB13" s="72" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BC13" s="96" t="s">
         <v>95</v>
@@ -8798,12 +8795,12 @@
     </row>
     <row r="14" spans="4:101" ht="24" x14ac:dyDescent="0.3">
       <c r="D14" s="60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E14" s="102"/>
       <c r="F14" s="102"/>
       <c r="M14" s="60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N14" s="102"/>
       <c r="O14" s="102"/>
@@ -8814,12 +8811,12 @@
       <c r="T14" s="70"/>
       <c r="U14" s="70"/>
       <c r="X14" s="60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Y14" s="102"/>
       <c r="Z14" s="102"/>
       <c r="AF14" s="60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AG14" s="102"/>
       <c r="AH14" s="102"/>
@@ -8844,7 +8841,7 @@
         <v>102</v>
       </c>
       <c r="BB14" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BC14" s="18" t="s">
         <v>2</v>
@@ -8976,7 +8973,7 @@
         <v>103</v>
       </c>
       <c r="BB15" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BC15" s="6" t="s">
         <v>4</v>
@@ -9112,7 +9109,7 @@
         <v>102</v>
       </c>
       <c r="BB16" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BC16" s="6" t="s">
         <v>5</v>
@@ -9212,41 +9209,41 @@
     </row>
     <row r="17" spans="4:101" ht="24" x14ac:dyDescent="0.3">
       <c r="D17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E17" s="102"/>
       <c r="F17" s="54"/>
       <c r="H17" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I17" s="102"/>
       <c r="J17" s="54"/>
       <c r="M17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N17" s="102"/>
       <c r="Q17" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R17" s="102"/>
       <c r="X17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Y17" s="102"/>
       <c r="Z17" s="54"/>
       <c r="AB17" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AC17" s="102"/>
       <c r="AD17" s="54"/>
       <c r="AE17" s="70"/>
       <c r="AF17" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AG17" s="102"/>
       <c r="AH17" s="54"/>
       <c r="AJ17" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AK17" s="102"/>
       <c r="AL17" s="54"/>
@@ -9267,7 +9264,7 @@
         <v>103</v>
       </c>
       <c r="BB17" s="57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BC17" s="7" t="s">
         <v>6</v>
@@ -9364,10 +9361,10 @@
         <v>35</v>
       </c>
       <c r="BI18" s="89" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BR18" s="89" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BW18" s="30" t="s">
         <v>14</v>
@@ -9388,7 +9385,7 @@
         <v>10</v>
       </c>
       <c r="CE18" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="CO18" s="30" t="s">
         <v>14</v>
@@ -9593,10 +9590,10 @@
         <v>1.3</v>
       </c>
       <c r="AZ20" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="CE20" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9692,7 +9689,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AZ21" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="BC21" s="58"/>
       <c r="BD21" s="58"/>
@@ -9706,7 +9703,7 @@
         <v>116</v>
       </c>
       <c r="CP21" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9768,7 +9765,7 @@
         <v>13</v>
       </c>
       <c r="AG22" s="109" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AH22" s="6" t="s">
         <v>4</v>
@@ -9795,7 +9792,7 @@
         <v>32</v>
       </c>
       <c r="AZ22" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="BW22" s="58" t="s">
         <v>120</v>
@@ -9804,7 +9801,7 @@
         <v>140</v>
       </c>
       <c r="CE22" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -9830,7 +9827,7 @@
         <v>13</v>
       </c>
       <c r="N23" s="104" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O23" s="104" t="s">
         <v>2</v>
@@ -9921,7 +9918,7 @@
         <v>13</v>
       </c>
       <c r="R24" s="104" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S24" s="104" t="s">
         <v>2</v>
@@ -9948,13 +9945,13 @@
         <v>13</v>
       </c>
       <c r="AK24" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AL24" s="29" t="s">
         <v>4</v>
       </c>
       <c r="BW24" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="CA24" s="1" t="s">
         <v>60</v>
@@ -9982,7 +9979,7 @@
         <v>14</v>
       </c>
       <c r="N25" s="105" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O25" s="105" t="s">
         <v>6</v>
@@ -10009,7 +10006,7 @@
         <v>14</v>
       </c>
       <c r="AG25" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AH25" s="7" t="s">
         <v>6</v>
@@ -10018,13 +10015,13 @@
         <v>13</v>
       </c>
       <c r="AK25" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AL25" s="29" t="s">
         <v>4</v>
       </c>
       <c r="AP25" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="CA25" s="1" t="s">
         <v>118</v>
@@ -10047,7 +10044,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>5</v>
@@ -10056,7 +10053,7 @@
         <v>14</v>
       </c>
       <c r="N26" s="105" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O26" s="105" t="s">
         <v>6</v>
@@ -10071,7 +10068,7 @@
         <v>6</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB26" s="30" t="s">
         <v>14</v>
@@ -10092,7 +10089,7 @@
         <v>5</v>
       </c>
       <c r="BW26" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10110,7 +10107,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J27" s="34" t="s">
         <v>6</v>
@@ -10129,7 +10126,7 @@
         <v>14</v>
       </c>
       <c r="R27" s="105" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S27" s="105" t="s">
         <v>6</v>
@@ -10153,7 +10150,7 @@
         <v>5</v>
       </c>
       <c r="CE27" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10175,7 +10172,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="107" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O28" s="107" t="s">
         <v>6</v>
@@ -10184,16 +10181,16 @@
         <v>14</v>
       </c>
       <c r="R28" s="105" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S28" s="105" t="s">
         <v>6</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF28" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AJ28" s="30" t="s">
         <v>14</v>
@@ -10205,10 +10202,10 @@
         <v>5</v>
       </c>
       <c r="BW28" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BY28" s="58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10221,7 +10218,7 @@
         <v>15</v>
       </c>
       <c r="N29" s="107" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O29" s="107" t="s">
         <v>6</v>
@@ -10230,7 +10227,7 @@
         <v>14</v>
       </c>
       <c r="R29" s="105" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S29" s="105" t="s">
         <v>6</v>
@@ -10245,15 +10242,15 @@
         <v>5</v>
       </c>
       <c r="BW29" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="CE29" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="30" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G30" s="70"/>
       <c r="H30" s="70"/>
@@ -10264,7 +10261,7 @@
         <v>15</v>
       </c>
       <c r="N30" s="108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O30" s="108" t="s">
         <v>6</v>
@@ -10282,19 +10279,19 @@
         <v>99</v>
       </c>
       <c r="AF30" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AJ30" s="30" t="s">
         <v>14</v>
       </c>
       <c r="AK30" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL30" s="30" t="s">
         <v>6</v>
       </c>
       <c r="CE30" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="CO30" s="1" t="s">
         <v>115</v>
@@ -10310,7 +10307,7 @@
         <v>15</v>
       </c>
       <c r="R31" s="107" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S31" s="107" t="s">
         <v>6</v>
@@ -10319,13 +10316,13 @@
         <v>82</v>
       </c>
       <c r="AB31" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AJ31" s="30" t="s">
         <v>14</v>
       </c>
       <c r="AK31" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL31" s="30" t="s">
         <v>6</v>
@@ -10333,16 +10330,16 @@
     </row>
     <row r="32" spans="4:101" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q32" s="107" t="s">
         <v>15</v>
       </c>
       <c r="R32" s="107" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S32" s="107" t="s">
         <v>6</v>
@@ -10351,7 +10348,7 @@
         <v>83</v>
       </c>
       <c r="AB32" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AF32" s="1" t="s">
         <v>99</v>
@@ -10360,7 +10357,7 @@
         <v>14</v>
       </c>
       <c r="AK32" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL32" s="30" t="s">
         <v>6</v>
@@ -10374,7 +10371,7 @@
         <v>15</v>
       </c>
       <c r="R33" s="107" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S33" s="107" t="s">
         <v>6</v>
@@ -10386,7 +10383,7 @@
         <v>14</v>
       </c>
       <c r="AK33" s="34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL33" s="34" t="s">
         <v>6</v>
@@ -10394,16 +10391,16 @@
     </row>
     <row r="34" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D34" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q34" s="108" t="s">
         <v>15</v>
       </c>
       <c r="R34" s="108" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S34" s="108" t="s">
         <v>6</v>
@@ -10425,16 +10422,16 @@
         <v>24</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="AJ36" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -10442,7 +10439,7 @@
         <v>25</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AF37" s="1" t="s">
         <v>79</v>
@@ -10453,18 +10450,18 @@
         <v>205</v>
       </c>
       <c r="AJ38" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="4:72" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D39" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="BT39" s="95" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="4:72" x14ac:dyDescent="0.2">
@@ -10474,7 +10471,7 @@
     </row>
     <row r="41" spans="4:72" x14ac:dyDescent="0.2">
       <c r="M41" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AJ41" s="1" t="s">
         <v>82</v>
@@ -10487,7 +10484,7 @@
     </row>
     <row r="43" spans="4:72" x14ac:dyDescent="0.2">
       <c r="M43" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="4:72" x14ac:dyDescent="0.2">

</xml_diff>